<commit_message>
- Conception : classes, maquettes, tests
</commit_message>
<xml_diff>
--- a/Planning_TPI_Chassot_Laurent.xlsx
+++ b/Planning_TPI_Chassot_Laurent.xlsx
@@ -15,11 +15,12 @@
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>Jour</t>
   </si>
@@ -1161,14 +1162,17 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1179,28 +1183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1210,6 +1193,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1249,7 +1250,7 @@
         <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1299,7 +1300,7 @@
         <xdr:cNvPr id="6" name="Image 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1684,9 +1685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FG90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O11" sqref="O11"/>
+      <selection pane="topRight" activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1698,16 +1699,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:162" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="118"/>
+      <c r="B1" s="107"/>
     </row>
     <row r="2" spans="1:162" x14ac:dyDescent="0.2">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="120"/>
+      <c r="B2" s="109"/>
     </row>
     <row r="3" spans="1:162" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
@@ -1732,206 +1733,206 @@
       <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="107" t="s">
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="109"/>
-      <c r="S6" s="107" t="s">
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+      <c r="O6" s="120"/>
+      <c r="P6" s="120"/>
+      <c r="Q6" s="120"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="108"/>
-      <c r="X6" s="108"/>
-      <c r="Y6" s="108"/>
-      <c r="Z6" s="109"/>
-      <c r="AA6" s="110" t="s">
+      <c r="T6" s="120"/>
+      <c r="U6" s="120"/>
+      <c r="V6" s="120"/>
+      <c r="W6" s="120"/>
+      <c r="X6" s="120"/>
+      <c r="Y6" s="120"/>
+      <c r="Z6" s="121"/>
+      <c r="AA6" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="AB6" s="111"/>
-      <c r="AC6" s="111"/>
-      <c r="AD6" s="111"/>
-      <c r="AE6" s="111"/>
-      <c r="AF6" s="111"/>
-      <c r="AG6" s="111"/>
-      <c r="AH6" s="112"/>
-      <c r="AI6" s="113" t="s">
+      <c r="AB6" s="112"/>
+      <c r="AC6" s="112"/>
+      <c r="AD6" s="112"/>
+      <c r="AE6" s="112"/>
+      <c r="AF6" s="112"/>
+      <c r="AG6" s="112"/>
+      <c r="AH6" s="113"/>
+      <c r="AI6" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="AJ6" s="108"/>
-      <c r="AK6" s="108"/>
-      <c r="AL6" s="108"/>
-      <c r="AM6" s="108"/>
-      <c r="AN6" s="108"/>
-      <c r="AO6" s="108"/>
-      <c r="AP6" s="109"/>
-      <c r="AQ6" s="107" t="s">
+      <c r="AJ6" s="120"/>
+      <c r="AK6" s="120"/>
+      <c r="AL6" s="120"/>
+      <c r="AM6" s="120"/>
+      <c r="AN6" s="120"/>
+      <c r="AO6" s="120"/>
+      <c r="AP6" s="121"/>
+      <c r="AQ6" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="AR6" s="108"/>
-      <c r="AS6" s="108"/>
-      <c r="AT6" s="108"/>
-      <c r="AU6" s="108"/>
-      <c r="AV6" s="108"/>
-      <c r="AW6" s="108"/>
-      <c r="AX6" s="109"/>
-      <c r="AY6" s="107" t="s">
+      <c r="AR6" s="120"/>
+      <c r="AS6" s="120"/>
+      <c r="AT6" s="120"/>
+      <c r="AU6" s="120"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
+      <c r="AX6" s="121"/>
+      <c r="AY6" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="AZ6" s="108"/>
-      <c r="BA6" s="108"/>
-      <c r="BB6" s="108"/>
-      <c r="BC6" s="108"/>
-      <c r="BD6" s="108"/>
-      <c r="BE6" s="108"/>
-      <c r="BF6" s="109"/>
-      <c r="BG6" s="107" t="s">
+      <c r="AZ6" s="120"/>
+      <c r="BA6" s="120"/>
+      <c r="BB6" s="120"/>
+      <c r="BC6" s="120"/>
+      <c r="BD6" s="120"/>
+      <c r="BE6" s="120"/>
+      <c r="BF6" s="121"/>
+      <c r="BG6" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="BH6" s="108"/>
-      <c r="BI6" s="108"/>
-      <c r="BJ6" s="108"/>
-      <c r="BK6" s="108"/>
-      <c r="BL6" s="108"/>
-      <c r="BM6" s="108"/>
-      <c r="BN6" s="109"/>
-      <c r="BO6" s="110" t="s">
+      <c r="BH6" s="120"/>
+      <c r="BI6" s="120"/>
+      <c r="BJ6" s="120"/>
+      <c r="BK6" s="120"/>
+      <c r="BL6" s="120"/>
+      <c r="BM6" s="120"/>
+      <c r="BN6" s="121"/>
+      <c r="BO6" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="BP6" s="111"/>
-      <c r="BQ6" s="111"/>
-      <c r="BR6" s="111"/>
-      <c r="BS6" s="111"/>
-      <c r="BT6" s="111"/>
-      <c r="BU6" s="111"/>
-      <c r="BV6" s="112"/>
-      <c r="BW6" s="113" t="s">
+      <c r="BP6" s="112"/>
+      <c r="BQ6" s="112"/>
+      <c r="BR6" s="112"/>
+      <c r="BS6" s="112"/>
+      <c r="BT6" s="112"/>
+      <c r="BU6" s="112"/>
+      <c r="BV6" s="113"/>
+      <c r="BW6" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="BX6" s="108"/>
-      <c r="BY6" s="108"/>
-      <c r="BZ6" s="108"/>
-      <c r="CA6" s="108"/>
-      <c r="CB6" s="108"/>
-      <c r="CC6" s="108"/>
-      <c r="CD6" s="109"/>
-      <c r="CE6" s="107" t="s">
+      <c r="BX6" s="120"/>
+      <c r="BY6" s="120"/>
+      <c r="BZ6" s="120"/>
+      <c r="CA6" s="120"/>
+      <c r="CB6" s="120"/>
+      <c r="CC6" s="120"/>
+      <c r="CD6" s="121"/>
+      <c r="CE6" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="CF6" s="108"/>
-      <c r="CG6" s="108"/>
-      <c r="CH6" s="108"/>
-      <c r="CI6" s="108"/>
-      <c r="CJ6" s="108"/>
-      <c r="CK6" s="108"/>
-      <c r="CL6" s="109"/>
-      <c r="CM6" s="107" t="s">
+      <c r="CF6" s="120"/>
+      <c r="CG6" s="120"/>
+      <c r="CH6" s="120"/>
+      <c r="CI6" s="120"/>
+      <c r="CJ6" s="120"/>
+      <c r="CK6" s="120"/>
+      <c r="CL6" s="121"/>
+      <c r="CM6" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="CN6" s="108"/>
-      <c r="CO6" s="108"/>
-      <c r="CP6" s="108"/>
-      <c r="CQ6" s="108"/>
-      <c r="CR6" s="108"/>
-      <c r="CS6" s="108"/>
-      <c r="CT6" s="109"/>
-      <c r="CU6" s="107" t="s">
+      <c r="CN6" s="120"/>
+      <c r="CO6" s="120"/>
+      <c r="CP6" s="120"/>
+      <c r="CQ6" s="120"/>
+      <c r="CR6" s="120"/>
+      <c r="CS6" s="120"/>
+      <c r="CT6" s="121"/>
+      <c r="CU6" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="CV6" s="108"/>
-      <c r="CW6" s="108"/>
-      <c r="CX6" s="108"/>
-      <c r="CY6" s="108"/>
-      <c r="CZ6" s="108"/>
-      <c r="DA6" s="108"/>
-      <c r="DB6" s="109"/>
-      <c r="DC6" s="110" t="s">
+      <c r="CV6" s="120"/>
+      <c r="CW6" s="120"/>
+      <c r="CX6" s="120"/>
+      <c r="CY6" s="120"/>
+      <c r="CZ6" s="120"/>
+      <c r="DA6" s="120"/>
+      <c r="DB6" s="121"/>
+      <c r="DC6" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="DD6" s="111"/>
-      <c r="DE6" s="111"/>
-      <c r="DF6" s="111"/>
-      <c r="DG6" s="111"/>
-      <c r="DH6" s="111"/>
-      <c r="DI6" s="111"/>
-      <c r="DJ6" s="112"/>
-      <c r="DK6" s="113" t="s">
+      <c r="DD6" s="112"/>
+      <c r="DE6" s="112"/>
+      <c r="DF6" s="112"/>
+      <c r="DG6" s="112"/>
+      <c r="DH6" s="112"/>
+      <c r="DI6" s="112"/>
+      <c r="DJ6" s="113"/>
+      <c r="DK6" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="DL6" s="108"/>
-      <c r="DM6" s="108"/>
-      <c r="DN6" s="108"/>
-      <c r="DO6" s="108"/>
-      <c r="DP6" s="108"/>
-      <c r="DQ6" s="108"/>
-      <c r="DR6" s="109"/>
-      <c r="DS6" s="107" t="s">
+      <c r="DL6" s="120"/>
+      <c r="DM6" s="120"/>
+      <c r="DN6" s="120"/>
+      <c r="DO6" s="120"/>
+      <c r="DP6" s="120"/>
+      <c r="DQ6" s="120"/>
+      <c r="DR6" s="121"/>
+      <c r="DS6" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="DT6" s="108"/>
-      <c r="DU6" s="108"/>
-      <c r="DV6" s="108"/>
-      <c r="DW6" s="108"/>
-      <c r="DX6" s="108"/>
-      <c r="DY6" s="108"/>
-      <c r="DZ6" s="109"/>
-      <c r="EA6" s="107" t="s">
+      <c r="DT6" s="120"/>
+      <c r="DU6" s="120"/>
+      <c r="DV6" s="120"/>
+      <c r="DW6" s="120"/>
+      <c r="DX6" s="120"/>
+      <c r="DY6" s="120"/>
+      <c r="DZ6" s="121"/>
+      <c r="EA6" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="EB6" s="108"/>
-      <c r="EC6" s="108"/>
-      <c r="ED6" s="108"/>
-      <c r="EE6" s="108"/>
-      <c r="EF6" s="108"/>
-      <c r="EG6" s="108"/>
-      <c r="EH6" s="109"/>
-      <c r="EI6" s="107" t="s">
+      <c r="EB6" s="120"/>
+      <c r="EC6" s="120"/>
+      <c r="ED6" s="120"/>
+      <c r="EE6" s="120"/>
+      <c r="EF6" s="120"/>
+      <c r="EG6" s="120"/>
+      <c r="EH6" s="121"/>
+      <c r="EI6" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="EJ6" s="108"/>
-      <c r="EK6" s="108"/>
-      <c r="EL6" s="108"/>
-      <c r="EM6" s="108"/>
-      <c r="EN6" s="108"/>
-      <c r="EO6" s="108"/>
-      <c r="EP6" s="109"/>
-      <c r="EQ6" s="110" t="s">
+      <c r="EJ6" s="120"/>
+      <c r="EK6" s="120"/>
+      <c r="EL6" s="120"/>
+      <c r="EM6" s="120"/>
+      <c r="EN6" s="120"/>
+      <c r="EO6" s="120"/>
+      <c r="EP6" s="121"/>
+      <c r="EQ6" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="ER6" s="111"/>
-      <c r="ES6" s="111"/>
-      <c r="ET6" s="111"/>
-      <c r="EU6" s="111"/>
-      <c r="EV6" s="111"/>
-      <c r="EW6" s="111"/>
-      <c r="EX6" s="112"/>
-      <c r="EY6" s="113" t="s">
+      <c r="ER6" s="112"/>
+      <c r="ES6" s="112"/>
+      <c r="ET6" s="112"/>
+      <c r="EU6" s="112"/>
+      <c r="EV6" s="112"/>
+      <c r="EW6" s="112"/>
+      <c r="EX6" s="113"/>
+      <c r="EY6" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="EZ6" s="108"/>
-      <c r="FA6" s="108"/>
-      <c r="FB6" s="108"/>
-      <c r="FC6" s="108"/>
-      <c r="FD6" s="108"/>
-      <c r="FE6" s="108"/>
-      <c r="FF6" s="109"/>
+      <c r="EZ6" s="120"/>
+      <c r="FA6" s="120"/>
+      <c r="FB6" s="120"/>
+      <c r="FC6" s="120"/>
+      <c r="FD6" s="120"/>
+      <c r="FE6" s="120"/>
+      <c r="FF6" s="121"/>
     </row>
     <row r="7" spans="1:162" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -3300,9 +3301,13 @@
         <v>57</v>
       </c>
       <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
+      <c r="T13" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
+      <c r="V13" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -3645,8 +3650,12 @@
       <c r="R15" s="9"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
+      <c r="U15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
@@ -3813,7 +3822,9 @@
         <v>57</v>
       </c>
       <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
+      <c r="T16" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
@@ -4309,7 +4320,9 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="9"/>
-      <c r="S19" s="80"/>
+      <c r="S19" s="80" t="s">
+        <v>57</v>
+      </c>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
@@ -4479,10 +4492,16 @@
       <c r="T20" s="84"/>
       <c r="U20" s="84"/>
       <c r="V20" s="84"/>
-      <c r="W20" s="84"/>
+      <c r="W20" s="84" t="s">
+        <v>57</v>
+      </c>
       <c r="X20" s="84"/>
-      <c r="Y20" s="84"/>
-      <c r="Z20" s="85"/>
+      <c r="Y20" s="84" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z20" s="85" t="s">
+        <v>57</v>
+      </c>
       <c r="AA20" s="93"/>
       <c r="AB20" s="76"/>
       <c r="AC20" s="76"/>
@@ -4493,11 +4512,21 @@
       <c r="AH20" s="94"/>
       <c r="AI20" s="83"/>
       <c r="AJ20" s="84"/>
-      <c r="AK20" s="84"/>
-      <c r="AL20" s="84"/>
-      <c r="AM20" s="84"/>
-      <c r="AN20" s="5"/>
-      <c r="AO20" s="5"/>
+      <c r="AK20" s="84" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL20" s="84" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM20" s="84" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO20" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="AP20" s="9"/>
       <c r="AQ20" s="22"/>
       <c r="AR20" s="23"/>
@@ -4645,7 +4674,9 @@
       <c r="T21" s="5"/>
       <c r="U21" s="88"/>
       <c r="V21" s="88"/>
-      <c r="W21" s="23"/>
+      <c r="W21" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="X21" s="23"/>
       <c r="Y21" s="5"/>
       <c r="Z21" s="9"/>
@@ -4812,8 +4843,12 @@
       <c r="U22" s="5"/>
       <c r="V22" s="88"/>
       <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
+      <c r="X22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y22" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="Z22" s="55"/>
       <c r="AA22" s="93"/>
       <c r="AB22" s="76"/>
@@ -4979,7 +5014,9 @@
       <c r="W23" s="88"/>
       <c r="X23" s="88"/>
       <c r="Y23" s="88"/>
-      <c r="Z23" s="89"/>
+      <c r="Z23" s="89" t="s">
+        <v>57</v>
+      </c>
       <c r="AA23" s="93"/>
       <c r="AB23" s="76"/>
       <c r="AC23" s="76"/>
@@ -4988,9 +5025,15 @@
       <c r="AF23" s="76"/>
       <c r="AG23" s="76"/>
       <c r="AH23" s="94"/>
-      <c r="AI23" s="7"/>
-      <c r="AJ23" s="5"/>
-      <c r="AK23" s="5"/>
+      <c r="AI23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK23" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="AL23" s="5"/>
       <c r="AM23" s="5"/>
       <c r="AN23" s="5"/>
@@ -5160,9 +5203,15 @@
       <c r="AL24" s="5"/>
       <c r="AM24" s="5"/>
       <c r="AN24" s="5"/>
-      <c r="AO24" s="5"/>
-      <c r="AP24" s="9"/>
-      <c r="AQ24" s="8"/>
+      <c r="AO24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ24" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="AR24" s="5"/>
       <c r="AS24" s="5"/>
       <c r="AT24" s="5"/>
@@ -5329,9 +5378,15 @@
       <c r="AO25" s="5"/>
       <c r="AP25" s="9"/>
       <c r="AQ25" s="7"/>
-      <c r="AR25" s="5"/>
-      <c r="AS25" s="5"/>
-      <c r="AT25" s="5"/>
+      <c r="AR25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT25" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="AU25" s="5"/>
       <c r="AV25" s="5"/>
       <c r="AW25" s="5"/>
@@ -5498,8 +5553,12 @@
       <c r="AR26" s="5"/>
       <c r="AS26" s="5"/>
       <c r="AT26" s="5"/>
-      <c r="AU26" s="5"/>
-      <c r="AV26" s="5"/>
+      <c r="AU26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV26" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="AW26" s="5"/>
       <c r="AX26" s="9"/>
       <c r="AY26" s="7"/>
@@ -5665,8 +5724,12 @@
       <c r="AS27" s="5"/>
       <c r="AT27" s="5"/>
       <c r="AU27" s="5"/>
-      <c r="AV27" s="5"/>
-      <c r="AW27" s="5"/>
+      <c r="AV27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW27" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="AX27" s="9"/>
       <c r="AY27" s="7"/>
       <c r="AZ27" s="5"/>
@@ -6161,8 +6224,12 @@
       <c r="AT30" s="23"/>
       <c r="AU30" s="5"/>
       <c r="AV30" s="5"/>
-      <c r="AW30" s="5"/>
-      <c r="AX30" s="9"/>
+      <c r="AW30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX30" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="AY30" s="27"/>
       <c r="AZ30" s="23"/>
       <c r="BA30" s="23"/>
@@ -9592,8 +9659,8 @@
       <c r="FF50" s="94"/>
     </row>
     <row r="51" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A51" s="116"/>
-      <c r="B51" s="117"/>
+      <c r="A51" s="114"/>
+      <c r="B51" s="123"/>
       <c r="C51" s="8"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -9920,8 +9987,8 @@
       <c r="FF52" s="94"/>
     </row>
     <row r="53" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A53" s="116"/>
-      <c r="B53" s="121"/>
+      <c r="A53" s="114"/>
+      <c r="B53" s="115"/>
       <c r="C53" s="8"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -10084,8 +10151,8 @@
       <c r="FF53" s="94"/>
     </row>
     <row r="54" spans="1:163" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="122"/>
-      <c r="B54" s="123"/>
+      <c r="A54" s="116"/>
+      <c r="B54" s="117"/>
       <c r="C54" s="11"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -10248,8 +10315,8 @@
       <c r="FF54" s="98"/>
     </row>
     <row r="55" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A55" s="115"/>
-      <c r="B55" s="115"/>
+      <c r="A55" s="118"/>
+      <c r="B55" s="118"/>
       <c r="C55" s="31"/>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
@@ -10413,8 +10480,8 @@
       <c r="FG55" s="100"/>
     </row>
     <row r="56" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A56" s="114"/>
-      <c r="B56" s="114"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="110"/>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
@@ -10578,8 +10645,8 @@
       <c r="FG56" s="100"/>
     </row>
     <row r="57" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A57" s="114"/>
-      <c r="B57" s="114"/>
+      <c r="A57" s="110"/>
+      <c r="B57" s="110"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
@@ -10743,8 +10810,8 @@
       <c r="FG57" s="100"/>
     </row>
     <row r="58" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A58" s="114"/>
-      <c r="B58" s="114"/>
+      <c r="A58" s="110"/>
+      <c r="B58" s="110"/>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
       <c r="E58" s="31"/>
@@ -10908,8 +10975,8 @@
       <c r="FG58" s="100"/>
     </row>
     <row r="59" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A59" s="114"/>
-      <c r="B59" s="114"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="110"/>
       <c r="C59" s="31"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
@@ -11073,8 +11140,8 @@
       <c r="FG59" s="100"/>
     </row>
     <row r="60" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A60" s="114"/>
-      <c r="B60" s="114"/>
+      <c r="A60" s="110"/>
+      <c r="B60" s="110"/>
       <c r="C60" s="31"/>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
@@ -11238,8 +11305,8 @@
       <c r="FG60" s="100"/>
     </row>
     <row r="61" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A61" s="114"/>
-      <c r="B61" s="114"/>
+      <c r="A61" s="110"/>
+      <c r="B61" s="110"/>
       <c r="C61" s="31"/>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
@@ -11403,8 +11470,8 @@
       <c r="FG61" s="100"/>
     </row>
     <row r="62" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A62" s="115"/>
-      <c r="B62" s="115"/>
+      <c r="A62" s="118"/>
+      <c r="B62" s="118"/>
       <c r="C62" s="31"/>
       <c r="D62" s="31"/>
       <c r="E62" s="31"/>
@@ -11568,8 +11635,8 @@
       <c r="FG62" s="100"/>
     </row>
     <row r="63" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A63" s="114"/>
-      <c r="B63" s="114"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="110"/>
       <c r="C63" s="31"/>
       <c r="D63" s="31"/>
       <c r="E63" s="31"/>
@@ -11733,8 +11800,8 @@
       <c r="FG63" s="100"/>
     </row>
     <row r="64" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A64" s="114"/>
-      <c r="B64" s="114"/>
+      <c r="A64" s="110"/>
+      <c r="B64" s="110"/>
       <c r="C64" s="31"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31"/>
@@ -11898,8 +11965,8 @@
       <c r="FG64" s="100"/>
     </row>
     <row r="65" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A65" s="114"/>
-      <c r="B65" s="114"/>
+      <c r="A65" s="110"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="31"/>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
@@ -12063,8 +12130,8 @@
       <c r="FG65" s="100"/>
     </row>
     <row r="66" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A66" s="114"/>
-      <c r="B66" s="114"/>
+      <c r="A66" s="110"/>
+      <c r="B66" s="110"/>
       <c r="C66" s="31"/>
       <c r="D66" s="31"/>
       <c r="E66" s="31"/>
@@ -12228,8 +12295,8 @@
       <c r="FG66" s="100"/>
     </row>
     <row r="67" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A67" s="114"/>
-      <c r="B67" s="114"/>
+      <c r="A67" s="110"/>
+      <c r="B67" s="110"/>
       <c r="C67" s="31"/>
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
@@ -12393,8 +12460,8 @@
       <c r="FG67" s="100"/>
     </row>
     <row r="68" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A68" s="115"/>
-      <c r="B68" s="115"/>
+      <c r="A68" s="118"/>
+      <c r="B68" s="118"/>
       <c r="C68" s="31"/>
       <c r="D68" s="31"/>
       <c r="E68" s="31"/>
@@ -12558,8 +12625,8 @@
       <c r="FG68" s="100"/>
     </row>
     <row r="69" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A69" s="114"/>
-      <c r="B69" s="114"/>
+      <c r="A69" s="110"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="31"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
@@ -12723,8 +12790,8 @@
       <c r="FG69" s="100"/>
     </row>
     <row r="70" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A70" s="114"/>
-      <c r="B70" s="114"/>
+      <c r="A70" s="110"/>
+      <c r="B70" s="110"/>
       <c r="C70" s="31"/>
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
@@ -12888,8 +12955,8 @@
       <c r="FG70" s="100"/>
     </row>
     <row r="71" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A71" s="114"/>
-      <c r="B71" s="114"/>
+      <c r="A71" s="110"/>
+      <c r="B71" s="110"/>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
@@ -13053,8 +13120,8 @@
       <c r="FG71" s="100"/>
     </row>
     <row r="72" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A72" s="114"/>
-      <c r="B72" s="114"/>
+      <c r="A72" s="110"/>
+      <c r="B72" s="110"/>
       <c r="C72" s="31"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
@@ -13218,8 +13285,8 @@
       <c r="FG72" s="100"/>
     </row>
     <row r="73" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A73" s="114"/>
-      <c r="B73" s="114"/>
+      <c r="A73" s="110"/>
+      <c r="B73" s="110"/>
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
@@ -13383,8 +13450,8 @@
       <c r="FG73" s="100"/>
     </row>
     <row r="74" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A74" s="114"/>
-      <c r="B74" s="114"/>
+      <c r="A74" s="110"/>
+      <c r="B74" s="110"/>
       <c r="C74" s="31"/>
       <c r="D74" s="31"/>
       <c r="E74" s="31"/>
@@ -13548,8 +13615,8 @@
       <c r="FG74" s="100"/>
     </row>
     <row r="75" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A75" s="115"/>
-      <c r="B75" s="115"/>
+      <c r="A75" s="118"/>
+      <c r="B75" s="118"/>
       <c r="C75" s="31"/>
       <c r="D75" s="31"/>
       <c r="E75" s="31"/>
@@ -13713,8 +13780,8 @@
       <c r="FG75" s="100"/>
     </row>
     <row r="76" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A76" s="114"/>
-      <c r="B76" s="114"/>
+      <c r="A76" s="110"/>
+      <c r="B76" s="110"/>
       <c r="C76" s="31"/>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
@@ -13878,8 +13945,8 @@
       <c r="FG76" s="100"/>
     </row>
     <row r="77" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A77" s="114"/>
-      <c r="B77" s="114"/>
+      <c r="A77" s="110"/>
+      <c r="B77" s="110"/>
       <c r="C77" s="31"/>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
@@ -14043,8 +14110,8 @@
       <c r="FG77" s="100"/>
     </row>
     <row r="78" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A78" s="114"/>
-      <c r="B78" s="114"/>
+      <c r="A78" s="110"/>
+      <c r="B78" s="110"/>
       <c r="C78" s="31"/>
       <c r="D78" s="31"/>
       <c r="E78" s="31"/>
@@ -14208,8 +14275,8 @@
       <c r="FG78" s="100"/>
     </row>
     <row r="79" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A79" s="114"/>
-      <c r="B79" s="114"/>
+      <c r="A79" s="110"/>
+      <c r="B79" s="110"/>
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
@@ -14373,8 +14440,8 @@
       <c r="FG79" s="100"/>
     </row>
     <row r="80" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A80" s="114"/>
-      <c r="B80" s="114"/>
+      <c r="A80" s="110"/>
+      <c r="B80" s="110"/>
       <c r="C80" s="31"/>
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
@@ -14538,8 +14605,8 @@
       <c r="FG80" s="100"/>
     </row>
     <row r="81" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A81" s="115"/>
-      <c r="B81" s="115"/>
+      <c r="A81" s="118"/>
+      <c r="B81" s="118"/>
       <c r="C81" s="31"/>
       <c r="D81" s="31"/>
       <c r="E81" s="31"/>
@@ -14703,8 +14770,8 @@
       <c r="FG81" s="100"/>
     </row>
     <row r="82" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A82" s="114"/>
-      <c r="B82" s="114"/>
+      <c r="A82" s="110"/>
+      <c r="B82" s="110"/>
       <c r="C82" s="31"/>
       <c r="D82" s="31"/>
       <c r="E82" s="31"/>
@@ -14868,8 +14935,8 @@
       <c r="FG82" s="100"/>
     </row>
     <row r="83" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A83" s="114"/>
-      <c r="B83" s="114"/>
+      <c r="A83" s="110"/>
+      <c r="B83" s="110"/>
       <c r="C83" s="31"/>
       <c r="D83" s="31"/>
       <c r="E83" s="31"/>
@@ -15033,8 +15100,8 @@
       <c r="FG83" s="100"/>
     </row>
     <row r="84" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A84" s="114"/>
-      <c r="B84" s="114"/>
+      <c r="A84" s="110"/>
+      <c r="B84" s="110"/>
       <c r="C84" s="31"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
@@ -15198,8 +15265,8 @@
       <c r="FG84" s="100"/>
     </row>
     <row r="85" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A85" s="114"/>
-      <c r="B85" s="114"/>
+      <c r="A85" s="110"/>
+      <c r="B85" s="110"/>
       <c r="C85" s="31"/>
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
@@ -15363,8 +15430,8 @@
       <c r="FG85" s="100"/>
     </row>
     <row r="86" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A86" s="114"/>
-      <c r="B86" s="114"/>
+      <c r="A86" s="110"/>
+      <c r="B86" s="110"/>
       <c r="C86" s="31"/>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
@@ -15528,8 +15595,8 @@
       <c r="FG86" s="100"/>
     </row>
     <row r="87" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A87" s="114"/>
-      <c r="B87" s="114"/>
+      <c r="A87" s="110"/>
+      <c r="B87" s="110"/>
       <c r="C87" s="31"/>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
@@ -15693,8 +15760,8 @@
       <c r="FG87" s="100"/>
     </row>
     <row r="88" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A88" s="114"/>
-      <c r="B88" s="114"/>
+      <c r="A88" s="110"/>
+      <c r="B88" s="110"/>
       <c r="C88" s="31"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
@@ -15858,8 +15925,8 @@
       <c r="FG88" s="100"/>
     </row>
     <row r="89" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A89" s="114"/>
-      <c r="B89" s="114"/>
+      <c r="A89" s="110"/>
+      <c r="B89" s="110"/>
       <c r="C89" s="31"/>
       <c r="D89" s="31"/>
       <c r="E89" s="31"/>
@@ -16189,6 +16256,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="AQ6:AX6"/>
+    <mergeCell ref="AY6:BF6"/>
+    <mergeCell ref="BG6:BN6"/>
+    <mergeCell ref="BO6:BV6"/>
+    <mergeCell ref="BW6:CD6"/>
+    <mergeCell ref="EA6:EH6"/>
+    <mergeCell ref="EI6:EP6"/>
+    <mergeCell ref="EQ6:EX6"/>
+    <mergeCell ref="EY6:FF6"/>
+    <mergeCell ref="CM6:CT6"/>
+    <mergeCell ref="CU6:DB6"/>
+    <mergeCell ref="DC6:DJ6"/>
+    <mergeCell ref="DK6:DR6"/>
+    <mergeCell ref="DS6:DZ6"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="CE6:CL6"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="AI6:AP6"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="S6:Z6"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A89:B89"/>
@@ -16205,50 +16316,6 @@
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A63:B63"/>
-    <mergeCell ref="AI6:AP6"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="S6:Z6"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="CE6:CL6"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="EA6:EH6"/>
-    <mergeCell ref="EI6:EP6"/>
-    <mergeCell ref="EQ6:EX6"/>
-    <mergeCell ref="EY6:FF6"/>
-    <mergeCell ref="CM6:CT6"/>
-    <mergeCell ref="CU6:DB6"/>
-    <mergeCell ref="DC6:DJ6"/>
-    <mergeCell ref="DK6:DR6"/>
-    <mergeCell ref="DS6:DZ6"/>
-    <mergeCell ref="AQ6:AX6"/>
-    <mergeCell ref="AY6:BF6"/>
-    <mergeCell ref="BG6:BN6"/>
-    <mergeCell ref="BO6:BV6"/>
-    <mergeCell ref="BW6:CD6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.62992125984251968" bottom="0.43" header="0.23622047244094491" footer="0.17"/>

</xml_diff>

<commit_message>
- Conception : Test technologique (GetInfos)
</commit_message>
<xml_diff>
--- a/Planning_TPI_Chassot_Laurent.xlsx
+++ b/Planning_TPI_Chassot_Laurent.xlsx
@@ -15,12 +15,11 @@
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="65">
   <si>
     <t>Jour</t>
   </si>
@@ -1162,17 +1161,14 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1183,7 +1179,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1193,24 +1210,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1250,7 +1249,7 @@
         <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1299,7 @@
         <xdr:cNvPr id="6" name="Image 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1687,7 +1686,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R37" sqref="R37"/>
+      <selection pane="topRight" activeCell="AW27" sqref="AW27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1699,16 +1698,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:162" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="107"/>
+      <c r="B1" s="118"/>
     </row>
     <row r="2" spans="1:162" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="109"/>
+      <c r="B2" s="120"/>
     </row>
     <row r="3" spans="1:162" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
@@ -1733,206 +1732,206 @@
       <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="122" t="s">
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="120"/>
-      <c r="M6" s="120"/>
-      <c r="N6" s="120"/>
-      <c r="O6" s="120"/>
-      <c r="P6" s="120"/>
-      <c r="Q6" s="120"/>
-      <c r="R6" s="121"/>
-      <c r="S6" s="122" t="s">
+      <c r="L6" s="108"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="108"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="108"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="T6" s="120"/>
-      <c r="U6" s="120"/>
-      <c r="V6" s="120"/>
-      <c r="W6" s="120"/>
-      <c r="X6" s="120"/>
-      <c r="Y6" s="120"/>
-      <c r="Z6" s="121"/>
-      <c r="AA6" s="111" t="s">
+      <c r="T6" s="108"/>
+      <c r="U6" s="108"/>
+      <c r="V6" s="108"/>
+      <c r="W6" s="108"/>
+      <c r="X6" s="108"/>
+      <c r="Y6" s="108"/>
+      <c r="Z6" s="109"/>
+      <c r="AA6" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="AB6" s="112"/>
-      <c r="AC6" s="112"/>
-      <c r="AD6" s="112"/>
-      <c r="AE6" s="112"/>
-      <c r="AF6" s="112"/>
-      <c r="AG6" s="112"/>
-      <c r="AH6" s="113"/>
-      <c r="AI6" s="119" t="s">
+      <c r="AB6" s="111"/>
+      <c r="AC6" s="111"/>
+      <c r="AD6" s="111"/>
+      <c r="AE6" s="111"/>
+      <c r="AF6" s="111"/>
+      <c r="AG6" s="111"/>
+      <c r="AH6" s="112"/>
+      <c r="AI6" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="AJ6" s="120"/>
-      <c r="AK6" s="120"/>
-      <c r="AL6" s="120"/>
-      <c r="AM6" s="120"/>
-      <c r="AN6" s="120"/>
-      <c r="AO6" s="120"/>
-      <c r="AP6" s="121"/>
-      <c r="AQ6" s="122" t="s">
+      <c r="AJ6" s="108"/>
+      <c r="AK6" s="108"/>
+      <c r="AL6" s="108"/>
+      <c r="AM6" s="108"/>
+      <c r="AN6" s="108"/>
+      <c r="AO6" s="108"/>
+      <c r="AP6" s="109"/>
+      <c r="AQ6" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="AR6" s="120"/>
-      <c r="AS6" s="120"/>
-      <c r="AT6" s="120"/>
-      <c r="AU6" s="120"/>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
-      <c r="AX6" s="121"/>
-      <c r="AY6" s="122" t="s">
+      <c r="AR6" s="108"/>
+      <c r="AS6" s="108"/>
+      <c r="AT6" s="108"/>
+      <c r="AU6" s="108"/>
+      <c r="AV6" s="108"/>
+      <c r="AW6" s="108"/>
+      <c r="AX6" s="109"/>
+      <c r="AY6" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="AZ6" s="120"/>
-      <c r="BA6" s="120"/>
-      <c r="BB6" s="120"/>
-      <c r="BC6" s="120"/>
-      <c r="BD6" s="120"/>
-      <c r="BE6" s="120"/>
-      <c r="BF6" s="121"/>
-      <c r="BG6" s="122" t="s">
+      <c r="AZ6" s="108"/>
+      <c r="BA6" s="108"/>
+      <c r="BB6" s="108"/>
+      <c r="BC6" s="108"/>
+      <c r="BD6" s="108"/>
+      <c r="BE6" s="108"/>
+      <c r="BF6" s="109"/>
+      <c r="BG6" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="BH6" s="120"/>
-      <c r="BI6" s="120"/>
-      <c r="BJ6" s="120"/>
-      <c r="BK6" s="120"/>
-      <c r="BL6" s="120"/>
-      <c r="BM6" s="120"/>
-      <c r="BN6" s="121"/>
-      <c r="BO6" s="111" t="s">
+      <c r="BH6" s="108"/>
+      <c r="BI6" s="108"/>
+      <c r="BJ6" s="108"/>
+      <c r="BK6" s="108"/>
+      <c r="BL6" s="108"/>
+      <c r="BM6" s="108"/>
+      <c r="BN6" s="109"/>
+      <c r="BO6" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="BP6" s="112"/>
-      <c r="BQ6" s="112"/>
-      <c r="BR6" s="112"/>
-      <c r="BS6" s="112"/>
-      <c r="BT6" s="112"/>
-      <c r="BU6" s="112"/>
-      <c r="BV6" s="113"/>
-      <c r="BW6" s="119" t="s">
+      <c r="BP6" s="111"/>
+      <c r="BQ6" s="111"/>
+      <c r="BR6" s="111"/>
+      <c r="BS6" s="111"/>
+      <c r="BT6" s="111"/>
+      <c r="BU6" s="111"/>
+      <c r="BV6" s="112"/>
+      <c r="BW6" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="BX6" s="120"/>
-      <c r="BY6" s="120"/>
-      <c r="BZ6" s="120"/>
-      <c r="CA6" s="120"/>
-      <c r="CB6" s="120"/>
-      <c r="CC6" s="120"/>
-      <c r="CD6" s="121"/>
-      <c r="CE6" s="122" t="s">
+      <c r="BX6" s="108"/>
+      <c r="BY6" s="108"/>
+      <c r="BZ6" s="108"/>
+      <c r="CA6" s="108"/>
+      <c r="CB6" s="108"/>
+      <c r="CC6" s="108"/>
+      <c r="CD6" s="109"/>
+      <c r="CE6" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="CF6" s="120"/>
-      <c r="CG6" s="120"/>
-      <c r="CH6" s="120"/>
-      <c r="CI6" s="120"/>
-      <c r="CJ6" s="120"/>
-      <c r="CK6" s="120"/>
-      <c r="CL6" s="121"/>
-      <c r="CM6" s="122" t="s">
+      <c r="CF6" s="108"/>
+      <c r="CG6" s="108"/>
+      <c r="CH6" s="108"/>
+      <c r="CI6" s="108"/>
+      <c r="CJ6" s="108"/>
+      <c r="CK6" s="108"/>
+      <c r="CL6" s="109"/>
+      <c r="CM6" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="CN6" s="120"/>
-      <c r="CO6" s="120"/>
-      <c r="CP6" s="120"/>
-      <c r="CQ6" s="120"/>
-      <c r="CR6" s="120"/>
-      <c r="CS6" s="120"/>
-      <c r="CT6" s="121"/>
-      <c r="CU6" s="122" t="s">
+      <c r="CN6" s="108"/>
+      <c r="CO6" s="108"/>
+      <c r="CP6" s="108"/>
+      <c r="CQ6" s="108"/>
+      <c r="CR6" s="108"/>
+      <c r="CS6" s="108"/>
+      <c r="CT6" s="109"/>
+      <c r="CU6" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CV6" s="120"/>
-      <c r="CW6" s="120"/>
-      <c r="CX6" s="120"/>
-      <c r="CY6" s="120"/>
-      <c r="CZ6" s="120"/>
-      <c r="DA6" s="120"/>
-      <c r="DB6" s="121"/>
-      <c r="DC6" s="111" t="s">
+      <c r="CV6" s="108"/>
+      <c r="CW6" s="108"/>
+      <c r="CX6" s="108"/>
+      <c r="CY6" s="108"/>
+      <c r="CZ6" s="108"/>
+      <c r="DA6" s="108"/>
+      <c r="DB6" s="109"/>
+      <c r="DC6" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="DD6" s="112"/>
-      <c r="DE6" s="112"/>
-      <c r="DF6" s="112"/>
-      <c r="DG6" s="112"/>
-      <c r="DH6" s="112"/>
-      <c r="DI6" s="112"/>
-      <c r="DJ6" s="113"/>
-      <c r="DK6" s="119" t="s">
+      <c r="DD6" s="111"/>
+      <c r="DE6" s="111"/>
+      <c r="DF6" s="111"/>
+      <c r="DG6" s="111"/>
+      <c r="DH6" s="111"/>
+      <c r="DI6" s="111"/>
+      <c r="DJ6" s="112"/>
+      <c r="DK6" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="DL6" s="120"/>
-      <c r="DM6" s="120"/>
-      <c r="DN6" s="120"/>
-      <c r="DO6" s="120"/>
-      <c r="DP6" s="120"/>
-      <c r="DQ6" s="120"/>
-      <c r="DR6" s="121"/>
-      <c r="DS6" s="122" t="s">
+      <c r="DL6" s="108"/>
+      <c r="DM6" s="108"/>
+      <c r="DN6" s="108"/>
+      <c r="DO6" s="108"/>
+      <c r="DP6" s="108"/>
+      <c r="DQ6" s="108"/>
+      <c r="DR6" s="109"/>
+      <c r="DS6" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="DT6" s="120"/>
-      <c r="DU6" s="120"/>
-      <c r="DV6" s="120"/>
-      <c r="DW6" s="120"/>
-      <c r="DX6" s="120"/>
-      <c r="DY6" s="120"/>
-      <c r="DZ6" s="121"/>
-      <c r="EA6" s="122" t="s">
+      <c r="DT6" s="108"/>
+      <c r="DU6" s="108"/>
+      <c r="DV6" s="108"/>
+      <c r="DW6" s="108"/>
+      <c r="DX6" s="108"/>
+      <c r="DY6" s="108"/>
+      <c r="DZ6" s="109"/>
+      <c r="EA6" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="EB6" s="120"/>
-      <c r="EC6" s="120"/>
-      <c r="ED6" s="120"/>
-      <c r="EE6" s="120"/>
-      <c r="EF6" s="120"/>
-      <c r="EG6" s="120"/>
-      <c r="EH6" s="121"/>
-      <c r="EI6" s="122" t="s">
+      <c r="EB6" s="108"/>
+      <c r="EC6" s="108"/>
+      <c r="ED6" s="108"/>
+      <c r="EE6" s="108"/>
+      <c r="EF6" s="108"/>
+      <c r="EG6" s="108"/>
+      <c r="EH6" s="109"/>
+      <c r="EI6" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="EJ6" s="120"/>
-      <c r="EK6" s="120"/>
-      <c r="EL6" s="120"/>
-      <c r="EM6" s="120"/>
-      <c r="EN6" s="120"/>
-      <c r="EO6" s="120"/>
-      <c r="EP6" s="121"/>
-      <c r="EQ6" s="111" t="s">
+      <c r="EJ6" s="108"/>
+      <c r="EK6" s="108"/>
+      <c r="EL6" s="108"/>
+      <c r="EM6" s="108"/>
+      <c r="EN6" s="108"/>
+      <c r="EO6" s="108"/>
+      <c r="EP6" s="109"/>
+      <c r="EQ6" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="ER6" s="112"/>
-      <c r="ES6" s="112"/>
-      <c r="ET6" s="112"/>
-      <c r="EU6" s="112"/>
-      <c r="EV6" s="112"/>
-      <c r="EW6" s="112"/>
-      <c r="EX6" s="113"/>
-      <c r="EY6" s="119" t="s">
+      <c r="ER6" s="111"/>
+      <c r="ES6" s="111"/>
+      <c r="ET6" s="111"/>
+      <c r="EU6" s="111"/>
+      <c r="EV6" s="111"/>
+      <c r="EW6" s="111"/>
+      <c r="EX6" s="112"/>
+      <c r="EY6" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="EZ6" s="120"/>
-      <c r="FA6" s="120"/>
-      <c r="FB6" s="120"/>
-      <c r="FC6" s="120"/>
-      <c r="FD6" s="120"/>
-      <c r="FE6" s="120"/>
-      <c r="FF6" s="121"/>
+      <c r="EZ6" s="108"/>
+      <c r="FA6" s="108"/>
+      <c r="FB6" s="108"/>
+      <c r="FC6" s="108"/>
+      <c r="FD6" s="108"/>
+      <c r="FE6" s="108"/>
+      <c r="FF6" s="109"/>
     </row>
     <row r="7" spans="1:162" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -6230,12 +6229,24 @@
       <c r="AX30" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AY30" s="27"/>
-      <c r="AZ30" s="23"/>
-      <c r="BA30" s="23"/>
-      <c r="BB30" s="23"/>
-      <c r="BC30" s="23"/>
-      <c r="BD30" s="86"/>
+      <c r="AY30" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ30" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA30" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB30" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC30" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="BD30" s="86" t="s">
+        <v>57</v>
+      </c>
       <c r="BE30" s="86"/>
       <c r="BF30" s="87"/>
       <c r="BG30" s="103"/>
@@ -6568,8 +6579,12 @@
       <c r="BB32" s="5"/>
       <c r="BC32" s="5"/>
       <c r="BD32" s="5"/>
-      <c r="BE32" s="5"/>
-      <c r="BF32" s="9"/>
+      <c r="BE32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF32" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="BG32" s="7"/>
       <c r="BH32" s="5"/>
       <c r="BI32" s="5"/>
@@ -9659,8 +9674,8 @@
       <c r="FF50" s="94"/>
     </row>
     <row r="51" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A51" s="114"/>
-      <c r="B51" s="123"/>
+      <c r="A51" s="116"/>
+      <c r="B51" s="117"/>
       <c r="C51" s="8"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -9987,8 +10002,8 @@
       <c r="FF52" s="94"/>
     </row>
     <row r="53" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A53" s="114"/>
-      <c r="B53" s="115"/>
+      <c r="A53" s="116"/>
+      <c r="B53" s="121"/>
       <c r="C53" s="8"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -10151,8 +10166,8 @@
       <c r="FF53" s="94"/>
     </row>
     <row r="54" spans="1:163" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="116"/>
-      <c r="B54" s="117"/>
+      <c r="A54" s="122"/>
+      <c r="B54" s="123"/>
       <c r="C54" s="11"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -10315,8 +10330,8 @@
       <c r="FF54" s="98"/>
     </row>
     <row r="55" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A55" s="118"/>
-      <c r="B55" s="118"/>
+      <c r="A55" s="115"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="31"/>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
@@ -10480,8 +10495,8 @@
       <c r="FG55" s="100"/>
     </row>
     <row r="56" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A56" s="110"/>
-      <c r="B56" s="110"/>
+      <c r="A56" s="114"/>
+      <c r="B56" s="114"/>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
@@ -10645,8 +10660,8 @@
       <c r="FG56" s="100"/>
     </row>
     <row r="57" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A57" s="110"/>
-      <c r="B57" s="110"/>
+      <c r="A57" s="114"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
@@ -10810,8 +10825,8 @@
       <c r="FG57" s="100"/>
     </row>
     <row r="58" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A58" s="110"/>
-      <c r="B58" s="110"/>
+      <c r="A58" s="114"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
       <c r="E58" s="31"/>
@@ -10975,8 +10990,8 @@
       <c r="FG58" s="100"/>
     </row>
     <row r="59" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A59" s="110"/>
-      <c r="B59" s="110"/>
+      <c r="A59" s="114"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="31"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
@@ -11140,8 +11155,8 @@
       <c r="FG59" s="100"/>
     </row>
     <row r="60" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A60" s="110"/>
-      <c r="B60" s="110"/>
+      <c r="A60" s="114"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="31"/>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
@@ -11305,8 +11320,8 @@
       <c r="FG60" s="100"/>
     </row>
     <row r="61" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A61" s="110"/>
-      <c r="B61" s="110"/>
+      <c r="A61" s="114"/>
+      <c r="B61" s="114"/>
       <c r="C61" s="31"/>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
@@ -11470,8 +11485,8 @@
       <c r="FG61" s="100"/>
     </row>
     <row r="62" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A62" s="118"/>
-      <c r="B62" s="118"/>
+      <c r="A62" s="115"/>
+      <c r="B62" s="115"/>
       <c r="C62" s="31"/>
       <c r="D62" s="31"/>
       <c r="E62" s="31"/>
@@ -11635,8 +11650,8 @@
       <c r="FG62" s="100"/>
     </row>
     <row r="63" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A63" s="110"/>
-      <c r="B63" s="110"/>
+      <c r="A63" s="114"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="31"/>
       <c r="D63" s="31"/>
       <c r="E63" s="31"/>
@@ -11800,8 +11815,8 @@
       <c r="FG63" s="100"/>
     </row>
     <row r="64" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A64" s="110"/>
-      <c r="B64" s="110"/>
+      <c r="A64" s="114"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="31"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31"/>
@@ -11965,8 +11980,8 @@
       <c r="FG64" s="100"/>
     </row>
     <row r="65" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A65" s="110"/>
-      <c r="B65" s="110"/>
+      <c r="A65" s="114"/>
+      <c r="B65" s="114"/>
       <c r="C65" s="31"/>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
@@ -12130,8 +12145,8 @@
       <c r="FG65" s="100"/>
     </row>
     <row r="66" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A66" s="110"/>
-      <c r="B66" s="110"/>
+      <c r="A66" s="114"/>
+      <c r="B66" s="114"/>
       <c r="C66" s="31"/>
       <c r="D66" s="31"/>
       <c r="E66" s="31"/>
@@ -12295,8 +12310,8 @@
       <c r="FG66" s="100"/>
     </row>
     <row r="67" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A67" s="110"/>
-      <c r="B67" s="110"/>
+      <c r="A67" s="114"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="31"/>
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
@@ -12460,8 +12475,8 @@
       <c r="FG67" s="100"/>
     </row>
     <row r="68" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A68" s="118"/>
-      <c r="B68" s="118"/>
+      <c r="A68" s="115"/>
+      <c r="B68" s="115"/>
       <c r="C68" s="31"/>
       <c r="D68" s="31"/>
       <c r="E68" s="31"/>
@@ -12625,8 +12640,8 @@
       <c r="FG68" s="100"/>
     </row>
     <row r="69" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A69" s="110"/>
-      <c r="B69" s="110"/>
+      <c r="A69" s="114"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="31"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
@@ -12790,8 +12805,8 @@
       <c r="FG69" s="100"/>
     </row>
     <row r="70" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A70" s="110"/>
-      <c r="B70" s="110"/>
+      <c r="A70" s="114"/>
+      <c r="B70" s="114"/>
       <c r="C70" s="31"/>
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
@@ -12955,8 +12970,8 @@
       <c r="FG70" s="100"/>
     </row>
     <row r="71" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A71" s="110"/>
-      <c r="B71" s="110"/>
+      <c r="A71" s="114"/>
+      <c r="B71" s="114"/>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
@@ -13120,8 +13135,8 @@
       <c r="FG71" s="100"/>
     </row>
     <row r="72" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A72" s="110"/>
-      <c r="B72" s="110"/>
+      <c r="A72" s="114"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="31"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
@@ -13285,8 +13300,8 @@
       <c r="FG72" s="100"/>
     </row>
     <row r="73" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A73" s="110"/>
-      <c r="B73" s="110"/>
+      <c r="A73" s="114"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
@@ -13450,8 +13465,8 @@
       <c r="FG73" s="100"/>
     </row>
     <row r="74" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A74" s="110"/>
-      <c r="B74" s="110"/>
+      <c r="A74" s="114"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="31"/>
       <c r="D74" s="31"/>
       <c r="E74" s="31"/>
@@ -13615,8 +13630,8 @@
       <c r="FG74" s="100"/>
     </row>
     <row r="75" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A75" s="118"/>
-      <c r="B75" s="118"/>
+      <c r="A75" s="115"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="31"/>
       <c r="D75" s="31"/>
       <c r="E75" s="31"/>
@@ -13780,8 +13795,8 @@
       <c r="FG75" s="100"/>
     </row>
     <row r="76" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A76" s="110"/>
-      <c r="B76" s="110"/>
+      <c r="A76" s="114"/>
+      <c r="B76" s="114"/>
       <c r="C76" s="31"/>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
@@ -13945,8 +13960,8 @@
       <c r="FG76" s="100"/>
     </row>
     <row r="77" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A77" s="110"/>
-      <c r="B77" s="110"/>
+      <c r="A77" s="114"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="31"/>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
@@ -14110,8 +14125,8 @@
       <c r="FG77" s="100"/>
     </row>
     <row r="78" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A78" s="110"/>
-      <c r="B78" s="110"/>
+      <c r="A78" s="114"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="31"/>
       <c r="D78" s="31"/>
       <c r="E78" s="31"/>
@@ -14275,8 +14290,8 @@
       <c r="FG78" s="100"/>
     </row>
     <row r="79" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A79" s="110"/>
-      <c r="B79" s="110"/>
+      <c r="A79" s="114"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
@@ -14440,8 +14455,8 @@
       <c r="FG79" s="100"/>
     </row>
     <row r="80" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A80" s="110"/>
-      <c r="B80" s="110"/>
+      <c r="A80" s="114"/>
+      <c r="B80" s="114"/>
       <c r="C80" s="31"/>
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
@@ -14605,8 +14620,8 @@
       <c r="FG80" s="100"/>
     </row>
     <row r="81" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A81" s="118"/>
-      <c r="B81" s="118"/>
+      <c r="A81" s="115"/>
+      <c r="B81" s="115"/>
       <c r="C81" s="31"/>
       <c r="D81" s="31"/>
       <c r="E81" s="31"/>
@@ -14770,8 +14785,8 @@
       <c r="FG81" s="100"/>
     </row>
     <row r="82" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A82" s="110"/>
-      <c r="B82" s="110"/>
+      <c r="A82" s="114"/>
+      <c r="B82" s="114"/>
       <c r="C82" s="31"/>
       <c r="D82" s="31"/>
       <c r="E82" s="31"/>
@@ -14935,8 +14950,8 @@
       <c r="FG82" s="100"/>
     </row>
     <row r="83" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A83" s="110"/>
-      <c r="B83" s="110"/>
+      <c r="A83" s="114"/>
+      <c r="B83" s="114"/>
       <c r="C83" s="31"/>
       <c r="D83" s="31"/>
       <c r="E83" s="31"/>
@@ -15100,8 +15115,8 @@
       <c r="FG83" s="100"/>
     </row>
     <row r="84" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A84" s="110"/>
-      <c r="B84" s="110"/>
+      <c r="A84" s="114"/>
+      <c r="B84" s="114"/>
       <c r="C84" s="31"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
@@ -15265,8 +15280,8 @@
       <c r="FG84" s="100"/>
     </row>
     <row r="85" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A85" s="110"/>
-      <c r="B85" s="110"/>
+      <c r="A85" s="114"/>
+      <c r="B85" s="114"/>
       <c r="C85" s="31"/>
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
@@ -15430,8 +15445,8 @@
       <c r="FG85" s="100"/>
     </row>
     <row r="86" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A86" s="110"/>
-      <c r="B86" s="110"/>
+      <c r="A86" s="114"/>
+      <c r="B86" s="114"/>
       <c r="C86" s="31"/>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
@@ -15595,8 +15610,8 @@
       <c r="FG86" s="100"/>
     </row>
     <row r="87" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A87" s="110"/>
-      <c r="B87" s="110"/>
+      <c r="A87" s="114"/>
+      <c r="B87" s="114"/>
       <c r="C87" s="31"/>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
@@ -15760,8 +15775,8 @@
       <c r="FG87" s="100"/>
     </row>
     <row r="88" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A88" s="110"/>
-      <c r="B88" s="110"/>
+      <c r="A88" s="114"/>
+      <c r="B88" s="114"/>
       <c r="C88" s="31"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
@@ -15925,8 +15940,8 @@
       <c r="FG88" s="100"/>
     </row>
     <row r="89" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A89" s="110"/>
-      <c r="B89" s="110"/>
+      <c r="A89" s="114"/>
+      <c r="B89" s="114"/>
       <c r="C89" s="31"/>
       <c r="D89" s="31"/>
       <c r="E89" s="31"/>
@@ -16256,20 +16271,36 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="AQ6:AX6"/>
-    <mergeCell ref="AY6:BF6"/>
-    <mergeCell ref="BG6:BN6"/>
-    <mergeCell ref="BO6:BV6"/>
-    <mergeCell ref="BW6:CD6"/>
-    <mergeCell ref="EA6:EH6"/>
-    <mergeCell ref="EI6:EP6"/>
-    <mergeCell ref="EQ6:EX6"/>
-    <mergeCell ref="EY6:FF6"/>
-    <mergeCell ref="CM6:CT6"/>
-    <mergeCell ref="CU6:DB6"/>
-    <mergeCell ref="DC6:DJ6"/>
-    <mergeCell ref="DK6:DR6"/>
-    <mergeCell ref="DS6:DZ6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="AA6:AH6"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="AI6:AP6"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="S6:Z6"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A86:B86"/>
@@ -16286,36 +16317,20 @@
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="AI6:AP6"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="S6:Z6"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="AA6:AH6"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="EA6:EH6"/>
+    <mergeCell ref="EI6:EP6"/>
+    <mergeCell ref="EQ6:EX6"/>
+    <mergeCell ref="EY6:FF6"/>
+    <mergeCell ref="CM6:CT6"/>
+    <mergeCell ref="CU6:DB6"/>
+    <mergeCell ref="DC6:DJ6"/>
+    <mergeCell ref="DK6:DR6"/>
+    <mergeCell ref="DS6:DZ6"/>
+    <mergeCell ref="AQ6:AX6"/>
+    <mergeCell ref="AY6:BF6"/>
+    <mergeCell ref="BG6:BN6"/>
+    <mergeCell ref="BO6:BV6"/>
+    <mergeCell ref="BW6:CD6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.62992125984251968" bottom="0.43" header="0.23622047244094491" footer="0.17"/>

</xml_diff>

<commit_message>
- Impl. + Tests fonctionnels "classiques"
</commit_message>
<xml_diff>
--- a/Planning_TPI_Chassot_Laurent.xlsx
+++ b/Planning_TPI_Chassot_Laurent.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="65">
   <si>
     <t>Jour</t>
   </si>
@@ -1684,9 +1684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FG90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AW27" sqref="AW27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DM27" sqref="DM27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5568,7 +5568,6 @@
       <c r="BD26" s="5"/>
       <c r="BE26" s="5"/>
       <c r="BF26" s="9"/>
-      <c r="BG26" s="7"/>
       <c r="BH26" s="5"/>
       <c r="BI26" s="5"/>
       <c r="BJ26" s="5"/>
@@ -5904,9 +5903,15 @@
       <c r="BE28" s="5"/>
       <c r="BF28" s="9"/>
       <c r="BG28" s="7"/>
-      <c r="BH28" s="5"/>
-      <c r="BI28" s="5"/>
-      <c r="BJ28" s="5"/>
+      <c r="BH28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ28" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="BK28" s="5"/>
       <c r="BL28" s="5"/>
       <c r="BM28" s="5"/>
@@ -6073,8 +6078,12 @@
       <c r="BH29" s="5"/>
       <c r="BI29" s="5"/>
       <c r="BJ29" s="5"/>
-      <c r="BK29" s="5"/>
-      <c r="BL29" s="5"/>
+      <c r="BK29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BL29" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="BM29" s="5"/>
       <c r="BN29" s="9"/>
       <c r="BO29" s="7"/>
@@ -6255,18 +6264,42 @@
       <c r="BJ30" s="86"/>
       <c r="BK30" s="86"/>
       <c r="BL30" s="86"/>
-      <c r="BM30" s="86"/>
-      <c r="BN30" s="87"/>
-      <c r="BO30" s="103"/>
-      <c r="BP30" s="86"/>
-      <c r="BQ30" s="86"/>
-      <c r="BR30" s="86"/>
-      <c r="BS30" s="5"/>
-      <c r="BT30" s="5"/>
-      <c r="BU30" s="5"/>
-      <c r="BV30" s="9"/>
-      <c r="BW30" s="7"/>
-      <c r="BX30" s="5"/>
+      <c r="BM30" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="BN30" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="BO30" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="BP30" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="BQ30" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="BR30" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="BS30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BT30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BU30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BV30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BW30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="BX30" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="BY30" s="5"/>
       <c r="BZ30" s="5"/>
       <c r="CA30" s="5"/>
@@ -6434,7 +6467,9 @@
       <c r="BW31" s="7"/>
       <c r="BX31" s="5"/>
       <c r="BY31" s="5"/>
-      <c r="BZ31" s="5"/>
+      <c r="BZ31" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="CA31" s="5"/>
       <c r="CB31" s="5"/>
       <c r="CC31" s="5"/>
@@ -6585,7 +6620,9 @@
       <c r="BF32" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BG32" s="7"/>
+      <c r="BG32" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="BH32" s="5"/>
       <c r="BI32" s="5"/>
       <c r="BJ32" s="5"/>
@@ -6608,7 +6645,9 @@
       <c r="CA32" s="5"/>
       <c r="CB32" s="5"/>
       <c r="CC32" s="5"/>
-      <c r="CD32" s="9"/>
+      <c r="CD32" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="CE32" s="93"/>
       <c r="CF32" s="76"/>
       <c r="CG32" s="76"/>
@@ -6618,9 +6657,15 @@
       <c r="CK32" s="76"/>
       <c r="CL32" s="94"/>
       <c r="CM32" s="8"/>
-      <c r="CN32" s="5"/>
-      <c r="CO32" s="5"/>
-      <c r="CP32" s="5"/>
+      <c r="CN32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="CO32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="CP32" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="CQ32" s="5"/>
       <c r="CR32" s="5"/>
       <c r="CS32" s="5"/>
@@ -6769,7 +6814,9 @@
       <c r="BV33" s="9"/>
       <c r="BW33" s="7"/>
       <c r="BX33" s="5"/>
-      <c r="BY33" s="86"/>
+      <c r="BY33" s="86" t="s">
+        <v>57</v>
+      </c>
       <c r="BZ33" s="86"/>
       <c r="CA33" s="5"/>
       <c r="CB33" s="5"/>
@@ -6936,10 +6983,21 @@
       <c r="BW34" s="27"/>
       <c r="BX34" s="23"/>
       <c r="BY34" s="23"/>
-      <c r="CA34" s="86"/>
-      <c r="CB34" s="86"/>
-      <c r="CC34" s="86"/>
-      <c r="CD34" s="87"/>
+      <c r="BZ34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CA34" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CB34" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CC34" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CD34" s="87" t="s">
+        <v>57</v>
+      </c>
       <c r="CE34" s="93"/>
       <c r="CF34" s="76"/>
       <c r="CG34" s="76"/>
@@ -7113,7 +7171,9 @@
       <c r="CJ35" s="76"/>
       <c r="CK35" s="76"/>
       <c r="CL35" s="94"/>
-      <c r="CM35" s="80"/>
+      <c r="CM35" s="80" t="s">
+        <v>57</v>
+      </c>
       <c r="CN35" s="5"/>
       <c r="CO35" s="5"/>
       <c r="CP35" s="5"/>
@@ -7282,17 +7342,39 @@
       <c r="CN36" s="5"/>
       <c r="CO36" s="5"/>
       <c r="CP36" s="5"/>
-      <c r="CQ36" s="5"/>
-      <c r="CR36" s="86"/>
-      <c r="CS36" s="86"/>
-      <c r="CT36" s="87"/>
-      <c r="CU36" s="103"/>
-      <c r="CV36" s="86"/>
-      <c r="CW36" s="86"/>
-      <c r="CX36" s="86"/>
-      <c r="CY36" s="86"/>
-      <c r="CZ36" s="5"/>
-      <c r="DA36" s="5"/>
+      <c r="CQ36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="CR36" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CS36" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CT36" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="CU36" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="CV36" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CW36" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CX36" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CY36" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="CZ36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DA36" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="DB36" s="9"/>
       <c r="DC36" s="7"/>
       <c r="DD36" s="5"/>
@@ -7460,12 +7542,20 @@
       <c r="CZ37" s="86"/>
       <c r="DA37" s="86"/>
       <c r="DB37" s="87"/>
-      <c r="DC37" s="103"/>
+      <c r="DC37" s="103" t="s">
+        <v>57</v>
+      </c>
       <c r="DD37" s="5"/>
       <c r="DE37" s="5"/>
-      <c r="DF37" s="5"/>
-      <c r="DG37" s="5"/>
-      <c r="DH37" s="5"/>
+      <c r="DF37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DG37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DH37" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="DI37" s="5"/>
       <c r="DJ37" s="9"/>
       <c r="DK37" s="7"/>
@@ -7625,9 +7715,13 @@
       <c r="CY38" s="23"/>
       <c r="CZ38" s="5"/>
       <c r="DA38" s="5"/>
-      <c r="DB38" s="9"/>
+      <c r="DB38" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="DC38" s="7"/>
-      <c r="DD38" s="77"/>
+      <c r="DD38" s="77" t="s">
+        <v>57</v>
+      </c>
       <c r="DE38" s="23"/>
       <c r="DF38" s="23"/>
       <c r="DG38" s="5"/>
@@ -7794,7 +7888,9 @@
       <c r="DB39" s="9"/>
       <c r="DC39" s="7"/>
       <c r="DD39" s="5"/>
-      <c r="DE39" s="86"/>
+      <c r="DE39" s="86" t="s">
+        <v>57</v>
+      </c>
       <c r="DF39" s="86"/>
       <c r="DG39" s="86"/>
       <c r="DH39" s="86"/>

</xml_diff>

<commit_message>
- Documentation : Tests spéciaux, corrections
</commit_message>
<xml_diff>
--- a/Planning_TPI_Chassot_Laurent.xlsx
+++ b/Planning_TPI_Chassot_Laurent.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="65">
   <si>
     <t>Jour</t>
   </si>
@@ -1161,14 +1161,17 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1179,28 +1182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1210,6 +1192,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1249,7 +1249,7 @@
         <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1299,7 +1299,7 @@
         <xdr:cNvPr id="6" name="Image 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1684,9 +1684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FG90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DM27" sqref="DM27"/>
+      <selection pane="topRight" activeCell="BR25" sqref="BR25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1698,16 +1698,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:162" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="118"/>
+      <c r="B1" s="107"/>
     </row>
     <row r="2" spans="1:162" x14ac:dyDescent="0.2">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="120"/>
+      <c r="B2" s="109"/>
     </row>
     <row r="3" spans="1:162" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
@@ -1732,206 +1732,206 @@
       <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="107" t="s">
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="109"/>
-      <c r="S6" s="107" t="s">
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+      <c r="O6" s="120"/>
+      <c r="P6" s="120"/>
+      <c r="Q6" s="120"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="108"/>
-      <c r="X6" s="108"/>
-      <c r="Y6" s="108"/>
-      <c r="Z6" s="109"/>
-      <c r="AA6" s="110" t="s">
+      <c r="T6" s="120"/>
+      <c r="U6" s="120"/>
+      <c r="V6" s="120"/>
+      <c r="W6" s="120"/>
+      <c r="X6" s="120"/>
+      <c r="Y6" s="120"/>
+      <c r="Z6" s="121"/>
+      <c r="AA6" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="AB6" s="111"/>
-      <c r="AC6" s="111"/>
-      <c r="AD6" s="111"/>
-      <c r="AE6" s="111"/>
-      <c r="AF6" s="111"/>
-      <c r="AG6" s="111"/>
-      <c r="AH6" s="112"/>
-      <c r="AI6" s="113" t="s">
+      <c r="AB6" s="112"/>
+      <c r="AC6" s="112"/>
+      <c r="AD6" s="112"/>
+      <c r="AE6" s="112"/>
+      <c r="AF6" s="112"/>
+      <c r="AG6" s="112"/>
+      <c r="AH6" s="113"/>
+      <c r="AI6" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="AJ6" s="108"/>
-      <c r="AK6" s="108"/>
-      <c r="AL6" s="108"/>
-      <c r="AM6" s="108"/>
-      <c r="AN6" s="108"/>
-      <c r="AO6" s="108"/>
-      <c r="AP6" s="109"/>
-      <c r="AQ6" s="107" t="s">
+      <c r="AJ6" s="120"/>
+      <c r="AK6" s="120"/>
+      <c r="AL6" s="120"/>
+      <c r="AM6" s="120"/>
+      <c r="AN6" s="120"/>
+      <c r="AO6" s="120"/>
+      <c r="AP6" s="121"/>
+      <c r="AQ6" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="AR6" s="108"/>
-      <c r="AS6" s="108"/>
-      <c r="AT6" s="108"/>
-      <c r="AU6" s="108"/>
-      <c r="AV6" s="108"/>
-      <c r="AW6" s="108"/>
-      <c r="AX6" s="109"/>
-      <c r="AY6" s="107" t="s">
+      <c r="AR6" s="120"/>
+      <c r="AS6" s="120"/>
+      <c r="AT6" s="120"/>
+      <c r="AU6" s="120"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="120"/>
+      <c r="AX6" s="121"/>
+      <c r="AY6" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="AZ6" s="108"/>
-      <c r="BA6" s="108"/>
-      <c r="BB6" s="108"/>
-      <c r="BC6" s="108"/>
-      <c r="BD6" s="108"/>
-      <c r="BE6" s="108"/>
-      <c r="BF6" s="109"/>
-      <c r="BG6" s="107" t="s">
+      <c r="AZ6" s="120"/>
+      <c r="BA6" s="120"/>
+      <c r="BB6" s="120"/>
+      <c r="BC6" s="120"/>
+      <c r="BD6" s="120"/>
+      <c r="BE6" s="120"/>
+      <c r="BF6" s="121"/>
+      <c r="BG6" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="BH6" s="108"/>
-      <c r="BI6" s="108"/>
-      <c r="BJ6" s="108"/>
-      <c r="BK6" s="108"/>
-      <c r="BL6" s="108"/>
-      <c r="BM6" s="108"/>
-      <c r="BN6" s="109"/>
-      <c r="BO6" s="110" t="s">
+      <c r="BH6" s="120"/>
+      <c r="BI6" s="120"/>
+      <c r="BJ6" s="120"/>
+      <c r="BK6" s="120"/>
+      <c r="BL6" s="120"/>
+      <c r="BM6" s="120"/>
+      <c r="BN6" s="121"/>
+      <c r="BO6" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="BP6" s="111"/>
-      <c r="BQ6" s="111"/>
-      <c r="BR6" s="111"/>
-      <c r="BS6" s="111"/>
-      <c r="BT6" s="111"/>
-      <c r="BU6" s="111"/>
-      <c r="BV6" s="112"/>
-      <c r="BW6" s="113" t="s">
+      <c r="BP6" s="112"/>
+      <c r="BQ6" s="112"/>
+      <c r="BR6" s="112"/>
+      <c r="BS6" s="112"/>
+      <c r="BT6" s="112"/>
+      <c r="BU6" s="112"/>
+      <c r="BV6" s="113"/>
+      <c r="BW6" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="BX6" s="108"/>
-      <c r="BY6" s="108"/>
-      <c r="BZ6" s="108"/>
-      <c r="CA6" s="108"/>
-      <c r="CB6" s="108"/>
-      <c r="CC6" s="108"/>
-      <c r="CD6" s="109"/>
-      <c r="CE6" s="107" t="s">
+      <c r="BX6" s="120"/>
+      <c r="BY6" s="120"/>
+      <c r="BZ6" s="120"/>
+      <c r="CA6" s="120"/>
+      <c r="CB6" s="120"/>
+      <c r="CC6" s="120"/>
+      <c r="CD6" s="121"/>
+      <c r="CE6" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="CF6" s="108"/>
-      <c r="CG6" s="108"/>
-      <c r="CH6" s="108"/>
-      <c r="CI6" s="108"/>
-      <c r="CJ6" s="108"/>
-      <c r="CK6" s="108"/>
-      <c r="CL6" s="109"/>
-      <c r="CM6" s="107" t="s">
+      <c r="CF6" s="120"/>
+      <c r="CG6" s="120"/>
+      <c r="CH6" s="120"/>
+      <c r="CI6" s="120"/>
+      <c r="CJ6" s="120"/>
+      <c r="CK6" s="120"/>
+      <c r="CL6" s="121"/>
+      <c r="CM6" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="CN6" s="108"/>
-      <c r="CO6" s="108"/>
-      <c r="CP6" s="108"/>
-      <c r="CQ6" s="108"/>
-      <c r="CR6" s="108"/>
-      <c r="CS6" s="108"/>
-      <c r="CT6" s="109"/>
-      <c r="CU6" s="107" t="s">
+      <c r="CN6" s="120"/>
+      <c r="CO6" s="120"/>
+      <c r="CP6" s="120"/>
+      <c r="CQ6" s="120"/>
+      <c r="CR6" s="120"/>
+      <c r="CS6" s="120"/>
+      <c r="CT6" s="121"/>
+      <c r="CU6" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="CV6" s="108"/>
-      <c r="CW6" s="108"/>
-      <c r="CX6" s="108"/>
-      <c r="CY6" s="108"/>
-      <c r="CZ6" s="108"/>
-      <c r="DA6" s="108"/>
-      <c r="DB6" s="109"/>
-      <c r="DC6" s="110" t="s">
+      <c r="CV6" s="120"/>
+      <c r="CW6" s="120"/>
+      <c r="CX6" s="120"/>
+      <c r="CY6" s="120"/>
+      <c r="CZ6" s="120"/>
+      <c r="DA6" s="120"/>
+      <c r="DB6" s="121"/>
+      <c r="DC6" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="DD6" s="111"/>
-      <c r="DE6" s="111"/>
-      <c r="DF6" s="111"/>
-      <c r="DG6" s="111"/>
-      <c r="DH6" s="111"/>
-      <c r="DI6" s="111"/>
-      <c r="DJ6" s="112"/>
-      <c r="DK6" s="113" t="s">
+      <c r="DD6" s="112"/>
+      <c r="DE6" s="112"/>
+      <c r="DF6" s="112"/>
+      <c r="DG6" s="112"/>
+      <c r="DH6" s="112"/>
+      <c r="DI6" s="112"/>
+      <c r="DJ6" s="113"/>
+      <c r="DK6" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="DL6" s="108"/>
-      <c r="DM6" s="108"/>
-      <c r="DN6" s="108"/>
-      <c r="DO6" s="108"/>
-      <c r="DP6" s="108"/>
-      <c r="DQ6" s="108"/>
-      <c r="DR6" s="109"/>
-      <c r="DS6" s="107" t="s">
+      <c r="DL6" s="120"/>
+      <c r="DM6" s="120"/>
+      <c r="DN6" s="120"/>
+      <c r="DO6" s="120"/>
+      <c r="DP6" s="120"/>
+      <c r="DQ6" s="120"/>
+      <c r="DR6" s="121"/>
+      <c r="DS6" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="DT6" s="108"/>
-      <c r="DU6" s="108"/>
-      <c r="DV6" s="108"/>
-      <c r="DW6" s="108"/>
-      <c r="DX6" s="108"/>
-      <c r="DY6" s="108"/>
-      <c r="DZ6" s="109"/>
-      <c r="EA6" s="107" t="s">
+      <c r="DT6" s="120"/>
+      <c r="DU6" s="120"/>
+      <c r="DV6" s="120"/>
+      <c r="DW6" s="120"/>
+      <c r="DX6" s="120"/>
+      <c r="DY6" s="120"/>
+      <c r="DZ6" s="121"/>
+      <c r="EA6" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="EB6" s="108"/>
-      <c r="EC6" s="108"/>
-      <c r="ED6" s="108"/>
-      <c r="EE6" s="108"/>
-      <c r="EF6" s="108"/>
-      <c r="EG6" s="108"/>
-      <c r="EH6" s="109"/>
-      <c r="EI6" s="107" t="s">
+      <c r="EB6" s="120"/>
+      <c r="EC6" s="120"/>
+      <c r="ED6" s="120"/>
+      <c r="EE6" s="120"/>
+      <c r="EF6" s="120"/>
+      <c r="EG6" s="120"/>
+      <c r="EH6" s="121"/>
+      <c r="EI6" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="EJ6" s="108"/>
-      <c r="EK6" s="108"/>
-      <c r="EL6" s="108"/>
-      <c r="EM6" s="108"/>
-      <c r="EN6" s="108"/>
-      <c r="EO6" s="108"/>
-      <c r="EP6" s="109"/>
-      <c r="EQ6" s="110" t="s">
+      <c r="EJ6" s="120"/>
+      <c r="EK6" s="120"/>
+      <c r="EL6" s="120"/>
+      <c r="EM6" s="120"/>
+      <c r="EN6" s="120"/>
+      <c r="EO6" s="120"/>
+      <c r="EP6" s="121"/>
+      <c r="EQ6" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="ER6" s="111"/>
-      <c r="ES6" s="111"/>
-      <c r="ET6" s="111"/>
-      <c r="EU6" s="111"/>
-      <c r="EV6" s="111"/>
-      <c r="EW6" s="111"/>
-      <c r="EX6" s="112"/>
-      <c r="EY6" s="113" t="s">
+      <c r="ER6" s="112"/>
+      <c r="ES6" s="112"/>
+      <c r="ET6" s="112"/>
+      <c r="EU6" s="112"/>
+      <c r="EV6" s="112"/>
+      <c r="EW6" s="112"/>
+      <c r="EX6" s="113"/>
+      <c r="EY6" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="EZ6" s="108"/>
-      <c r="FA6" s="108"/>
-      <c r="FB6" s="108"/>
-      <c r="FC6" s="108"/>
-      <c r="FD6" s="108"/>
-      <c r="FE6" s="108"/>
-      <c r="FF6" s="109"/>
+      <c r="EZ6" s="120"/>
+      <c r="FA6" s="120"/>
+      <c r="FB6" s="120"/>
+      <c r="FC6" s="120"/>
+      <c r="FD6" s="120"/>
+      <c r="FE6" s="120"/>
+      <c r="FF6" s="121"/>
     </row>
     <row r="7" spans="1:162" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -7556,14 +7556,30 @@
       <c r="DH37" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="DI37" s="5"/>
-      <c r="DJ37" s="9"/>
-      <c r="DK37" s="7"/>
-      <c r="DL37" s="5"/>
-      <c r="DM37" s="5"/>
-      <c r="DN37" s="5"/>
-      <c r="DO37" s="23"/>
-      <c r="DP37" s="23"/>
+      <c r="DI37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DJ37" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="DK37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="DL37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DM37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DN37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DO37" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="DP37" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="DQ37" s="23"/>
       <c r="DR37" s="24"/>
       <c r="DS37" s="27"/>
@@ -8068,8 +8084,12 @@
       <c r="DN40" s="23"/>
       <c r="DO40" s="23"/>
       <c r="DP40" s="23"/>
-      <c r="DQ40" s="23"/>
-      <c r="DR40" s="24"/>
+      <c r="DQ40" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="DR40" s="24" t="s">
+        <v>57</v>
+      </c>
       <c r="DS40" s="27"/>
       <c r="DT40" s="23"/>
       <c r="DU40" s="23"/>
@@ -9770,8 +9790,8 @@
       <c r="FF50" s="94"/>
     </row>
     <row r="51" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A51" s="116"/>
-      <c r="B51" s="117"/>
+      <c r="A51" s="114"/>
+      <c r="B51" s="123"/>
       <c r="C51" s="8"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -10098,8 +10118,8 @@
       <c r="FF52" s="94"/>
     </row>
     <row r="53" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A53" s="116"/>
-      <c r="B53" s="121"/>
+      <c r="A53" s="114"/>
+      <c r="B53" s="115"/>
       <c r="C53" s="8"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -10262,8 +10282,8 @@
       <c r="FF53" s="94"/>
     </row>
     <row r="54" spans="1:163" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="122"/>
-      <c r="B54" s="123"/>
+      <c r="A54" s="116"/>
+      <c r="B54" s="117"/>
       <c r="C54" s="11"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -10426,8 +10446,8 @@
       <c r="FF54" s="98"/>
     </row>
     <row r="55" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A55" s="115"/>
-      <c r="B55" s="115"/>
+      <c r="A55" s="118"/>
+      <c r="B55" s="118"/>
       <c r="C55" s="31"/>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
@@ -10591,8 +10611,8 @@
       <c r="FG55" s="100"/>
     </row>
     <row r="56" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A56" s="114"/>
-      <c r="B56" s="114"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="110"/>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
@@ -10756,8 +10776,8 @@
       <c r="FG56" s="100"/>
     </row>
     <row r="57" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A57" s="114"/>
-      <c r="B57" s="114"/>
+      <c r="A57" s="110"/>
+      <c r="B57" s="110"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
@@ -10921,8 +10941,8 @@
       <c r="FG57" s="100"/>
     </row>
     <row r="58" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A58" s="114"/>
-      <c r="B58" s="114"/>
+      <c r="A58" s="110"/>
+      <c r="B58" s="110"/>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
       <c r="E58" s="31"/>
@@ -11086,8 +11106,8 @@
       <c r="FG58" s="100"/>
     </row>
     <row r="59" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A59" s="114"/>
-      <c r="B59" s="114"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="110"/>
       <c r="C59" s="31"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
@@ -11251,8 +11271,8 @@
       <c r="FG59" s="100"/>
     </row>
     <row r="60" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A60" s="114"/>
-      <c r="B60" s="114"/>
+      <c r="A60" s="110"/>
+      <c r="B60" s="110"/>
       <c r="C60" s="31"/>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
@@ -11416,8 +11436,8 @@
       <c r="FG60" s="100"/>
     </row>
     <row r="61" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A61" s="114"/>
-      <c r="B61" s="114"/>
+      <c r="A61" s="110"/>
+      <c r="B61" s="110"/>
       <c r="C61" s="31"/>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
@@ -11581,8 +11601,8 @@
       <c r="FG61" s="100"/>
     </row>
     <row r="62" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A62" s="115"/>
-      <c r="B62" s="115"/>
+      <c r="A62" s="118"/>
+      <c r="B62" s="118"/>
       <c r="C62" s="31"/>
       <c r="D62" s="31"/>
       <c r="E62" s="31"/>
@@ -11746,8 +11766,8 @@
       <c r="FG62" s="100"/>
     </row>
     <row r="63" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A63" s="114"/>
-      <c r="B63" s="114"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="110"/>
       <c r="C63" s="31"/>
       <c r="D63" s="31"/>
       <c r="E63" s="31"/>
@@ -11911,8 +11931,8 @@
       <c r="FG63" s="100"/>
     </row>
     <row r="64" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A64" s="114"/>
-      <c r="B64" s="114"/>
+      <c r="A64" s="110"/>
+      <c r="B64" s="110"/>
       <c r="C64" s="31"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31"/>
@@ -12076,8 +12096,8 @@
       <c r="FG64" s="100"/>
     </row>
     <row r="65" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A65" s="114"/>
-      <c r="B65" s="114"/>
+      <c r="A65" s="110"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="31"/>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
@@ -12241,8 +12261,8 @@
       <c r="FG65" s="100"/>
     </row>
     <row r="66" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A66" s="114"/>
-      <c r="B66" s="114"/>
+      <c r="A66" s="110"/>
+      <c r="B66" s="110"/>
       <c r="C66" s="31"/>
       <c r="D66" s="31"/>
       <c r="E66" s="31"/>
@@ -12406,8 +12426,8 @@
       <c r="FG66" s="100"/>
     </row>
     <row r="67" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A67" s="114"/>
-      <c r="B67" s="114"/>
+      <c r="A67" s="110"/>
+      <c r="B67" s="110"/>
       <c r="C67" s="31"/>
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
@@ -12571,8 +12591,8 @@
       <c r="FG67" s="100"/>
     </row>
     <row r="68" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A68" s="115"/>
-      <c r="B68" s="115"/>
+      <c r="A68" s="118"/>
+      <c r="B68" s="118"/>
       <c r="C68" s="31"/>
       <c r="D68" s="31"/>
       <c r="E68" s="31"/>
@@ -12736,8 +12756,8 @@
       <c r="FG68" s="100"/>
     </row>
     <row r="69" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A69" s="114"/>
-      <c r="B69" s="114"/>
+      <c r="A69" s="110"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="31"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
@@ -12901,8 +12921,8 @@
       <c r="FG69" s="100"/>
     </row>
     <row r="70" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A70" s="114"/>
-      <c r="B70" s="114"/>
+      <c r="A70" s="110"/>
+      <c r="B70" s="110"/>
       <c r="C70" s="31"/>
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
@@ -13066,8 +13086,8 @@
       <c r="FG70" s="100"/>
     </row>
     <row r="71" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A71" s="114"/>
-      <c r="B71" s="114"/>
+      <c r="A71" s="110"/>
+      <c r="B71" s="110"/>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
@@ -13231,8 +13251,8 @@
       <c r="FG71" s="100"/>
     </row>
     <row r="72" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A72" s="114"/>
-      <c r="B72" s="114"/>
+      <c r="A72" s="110"/>
+      <c r="B72" s="110"/>
       <c r="C72" s="31"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
@@ -13396,8 +13416,8 @@
       <c r="FG72" s="100"/>
     </row>
     <row r="73" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A73" s="114"/>
-      <c r="B73" s="114"/>
+      <c r="A73" s="110"/>
+      <c r="B73" s="110"/>
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
@@ -13561,8 +13581,8 @@
       <c r="FG73" s="100"/>
     </row>
     <row r="74" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A74" s="114"/>
-      <c r="B74" s="114"/>
+      <c r="A74" s="110"/>
+      <c r="B74" s="110"/>
       <c r="C74" s="31"/>
       <c r="D74" s="31"/>
       <c r="E74" s="31"/>
@@ -13726,8 +13746,8 @@
       <c r="FG74" s="100"/>
     </row>
     <row r="75" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A75" s="115"/>
-      <c r="B75" s="115"/>
+      <c r="A75" s="118"/>
+      <c r="B75" s="118"/>
       <c r="C75" s="31"/>
       <c r="D75" s="31"/>
       <c r="E75" s="31"/>
@@ -13891,8 +13911,8 @@
       <c r="FG75" s="100"/>
     </row>
     <row r="76" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A76" s="114"/>
-      <c r="B76" s="114"/>
+      <c r="A76" s="110"/>
+      <c r="B76" s="110"/>
       <c r="C76" s="31"/>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
@@ -14056,8 +14076,8 @@
       <c r="FG76" s="100"/>
     </row>
     <row r="77" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A77" s="114"/>
-      <c r="B77" s="114"/>
+      <c r="A77" s="110"/>
+      <c r="B77" s="110"/>
       <c r="C77" s="31"/>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
@@ -14221,8 +14241,8 @@
       <c r="FG77" s="100"/>
     </row>
     <row r="78" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A78" s="114"/>
-      <c r="B78" s="114"/>
+      <c r="A78" s="110"/>
+      <c r="B78" s="110"/>
       <c r="C78" s="31"/>
       <c r="D78" s="31"/>
       <c r="E78" s="31"/>
@@ -14386,8 +14406,8 @@
       <c r="FG78" s="100"/>
     </row>
     <row r="79" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A79" s="114"/>
-      <c r="B79" s="114"/>
+      <c r="A79" s="110"/>
+      <c r="B79" s="110"/>
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
@@ -14551,8 +14571,8 @@
       <c r="FG79" s="100"/>
     </row>
     <row r="80" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A80" s="114"/>
-      <c r="B80" s="114"/>
+      <c r="A80" s="110"/>
+      <c r="B80" s="110"/>
       <c r="C80" s="31"/>
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
@@ -14716,8 +14736,8 @@
       <c r="FG80" s="100"/>
     </row>
     <row r="81" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A81" s="115"/>
-      <c r="B81" s="115"/>
+      <c r="A81" s="118"/>
+      <c r="B81" s="118"/>
       <c r="C81" s="31"/>
       <c r="D81" s="31"/>
       <c r="E81" s="31"/>
@@ -14881,8 +14901,8 @@
       <c r="FG81" s="100"/>
     </row>
     <row r="82" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A82" s="114"/>
-      <c r="B82" s="114"/>
+      <c r="A82" s="110"/>
+      <c r="B82" s="110"/>
       <c r="C82" s="31"/>
       <c r="D82" s="31"/>
       <c r="E82" s="31"/>
@@ -15046,8 +15066,8 @@
       <c r="FG82" s="100"/>
     </row>
     <row r="83" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A83" s="114"/>
-      <c r="B83" s="114"/>
+      <c r="A83" s="110"/>
+      <c r="B83" s="110"/>
       <c r="C83" s="31"/>
       <c r="D83" s="31"/>
       <c r="E83" s="31"/>
@@ -15211,8 +15231,8 @@
       <c r="FG83" s="100"/>
     </row>
     <row r="84" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A84" s="114"/>
-      <c r="B84" s="114"/>
+      <c r="A84" s="110"/>
+      <c r="B84" s="110"/>
       <c r="C84" s="31"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
@@ -15376,8 +15396,8 @@
       <c r="FG84" s="100"/>
     </row>
     <row r="85" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A85" s="114"/>
-      <c r="B85" s="114"/>
+      <c r="A85" s="110"/>
+      <c r="B85" s="110"/>
       <c r="C85" s="31"/>
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
@@ -15541,8 +15561,8 @@
       <c r="FG85" s="100"/>
     </row>
     <row r="86" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A86" s="114"/>
-      <c r="B86" s="114"/>
+      <c r="A86" s="110"/>
+      <c r="B86" s="110"/>
       <c r="C86" s="31"/>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
@@ -15706,8 +15726,8 @@
       <c r="FG86" s="100"/>
     </row>
     <row r="87" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A87" s="114"/>
-      <c r="B87" s="114"/>
+      <c r="A87" s="110"/>
+      <c r="B87" s="110"/>
       <c r="C87" s="31"/>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
@@ -15871,8 +15891,8 @@
       <c r="FG87" s="100"/>
     </row>
     <row r="88" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A88" s="114"/>
-      <c r="B88" s="114"/>
+      <c r="A88" s="110"/>
+      <c r="B88" s="110"/>
       <c r="C88" s="31"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
@@ -16036,8 +16056,8 @@
       <c r="FG88" s="100"/>
     </row>
     <row r="89" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A89" s="114"/>
-      <c r="B89" s="114"/>
+      <c r="A89" s="110"/>
+      <c r="B89" s="110"/>
       <c r="C89" s="31"/>
       <c r="D89" s="31"/>
       <c r="E89" s="31"/>
@@ -16367,6 +16387,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="AQ6:AX6"/>
+    <mergeCell ref="AY6:BF6"/>
+    <mergeCell ref="BG6:BN6"/>
+    <mergeCell ref="BO6:BV6"/>
+    <mergeCell ref="BW6:CD6"/>
+    <mergeCell ref="EA6:EH6"/>
+    <mergeCell ref="EI6:EP6"/>
+    <mergeCell ref="EQ6:EX6"/>
+    <mergeCell ref="EY6:FF6"/>
+    <mergeCell ref="CM6:CT6"/>
+    <mergeCell ref="CU6:DB6"/>
+    <mergeCell ref="DC6:DJ6"/>
+    <mergeCell ref="DK6:DR6"/>
+    <mergeCell ref="DS6:DZ6"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="CE6:CL6"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="AI6:AP6"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="S6:Z6"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A89:B89"/>
@@ -16383,50 +16447,6 @@
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A63:B63"/>
-    <mergeCell ref="AI6:AP6"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="S6:Z6"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="CE6:CL6"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="EA6:EH6"/>
-    <mergeCell ref="EI6:EP6"/>
-    <mergeCell ref="EQ6:EX6"/>
-    <mergeCell ref="EY6:FF6"/>
-    <mergeCell ref="CM6:CT6"/>
-    <mergeCell ref="CU6:DB6"/>
-    <mergeCell ref="DC6:DJ6"/>
-    <mergeCell ref="DK6:DR6"/>
-    <mergeCell ref="DS6:DZ6"/>
-    <mergeCell ref="AQ6:AX6"/>
-    <mergeCell ref="AY6:BF6"/>
-    <mergeCell ref="BG6:BN6"/>
-    <mergeCell ref="BO6:BV6"/>
-    <mergeCell ref="BW6:CD6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.62992125984251968" bottom="0.43" header="0.23622047244094491" footer="0.17"/>

</xml_diff>

<commit_message>
- Rapport terminé + manuel utilisateur
</commit_message>
<xml_diff>
--- a/Planning_TPI_Chassot_Laurent.xlsx
+++ b/Planning_TPI_Chassot_Laurent.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="65">
   <si>
     <t>Jour</t>
   </si>
@@ -237,6 +237,34 @@
     </r>
   </si>
   <si>
+    <t>Planning  - StreamScan</t>
+  </si>
+  <si>
+    <t>Réserves</t>
+  </si>
+  <si>
+    <r>
+      <t>Mise en page (design) [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>optionnel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="16"/>
@@ -286,27 +314,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Implémentation</t>
-    </r>
-  </si>
-  <si>
-    <t>Planning  - StreamScan</t>
-  </si>
-  <si>
-    <t>Réserves</t>
-  </si>
-  <si>
-    <r>
-      <t>Mise en page (design) [</t>
+      <t xml:space="preserve"> Implémentation | </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <sz val="16"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
       </rPr>
-      <t>optionnel</t>
+      <t>§</t>
     </r>
     <r>
       <rPr>
@@ -314,7 +331,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>]</t>
+      <t xml:space="preserve"> Autres</t>
     </r>
   </si>
 </sst>
@@ -322,7 +339,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -367,8 +384,14 @@
       <name val="Wingdings"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,6 +461,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF333333"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1161,6 +1190,27 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1218,6 +1268,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF333333"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1684,9 +1739,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FG90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BR25" sqref="BR25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DY37" sqref="DY37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1698,16 +1753,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:162" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="107"/>
+      <c r="B1" s="114"/>
     </row>
     <row r="2" spans="1:162" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="109"/>
+      <c r="B2" s="116"/>
     </row>
     <row r="3" spans="1:162" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
@@ -1716,13 +1771,13 @@
     </row>
     <row r="4" spans="1:162" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:162" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:162" x14ac:dyDescent="0.2">
@@ -1732,206 +1787,206 @@
       <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="122" t="s">
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="120"/>
-      <c r="M6" s="120"/>
-      <c r="N6" s="120"/>
-      <c r="O6" s="120"/>
-      <c r="P6" s="120"/>
-      <c r="Q6" s="120"/>
-      <c r="R6" s="121"/>
-      <c r="S6" s="122" t="s">
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="127"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="T6" s="120"/>
-      <c r="U6" s="120"/>
-      <c r="V6" s="120"/>
-      <c r="W6" s="120"/>
-      <c r="X6" s="120"/>
-      <c r="Y6" s="120"/>
-      <c r="Z6" s="121"/>
-      <c r="AA6" s="111" t="s">
+      <c r="T6" s="127"/>
+      <c r="U6" s="127"/>
+      <c r="V6" s="127"/>
+      <c r="W6" s="127"/>
+      <c r="X6" s="127"/>
+      <c r="Y6" s="127"/>
+      <c r="Z6" s="128"/>
+      <c r="AA6" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="AB6" s="112"/>
-      <c r="AC6" s="112"/>
-      <c r="AD6" s="112"/>
-      <c r="AE6" s="112"/>
-      <c r="AF6" s="112"/>
-      <c r="AG6" s="112"/>
-      <c r="AH6" s="113"/>
-      <c r="AI6" s="119" t="s">
+      <c r="AB6" s="119"/>
+      <c r="AC6" s="119"/>
+      <c r="AD6" s="119"/>
+      <c r="AE6" s="119"/>
+      <c r="AF6" s="119"/>
+      <c r="AG6" s="119"/>
+      <c r="AH6" s="120"/>
+      <c r="AI6" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="AJ6" s="120"/>
-      <c r="AK6" s="120"/>
-      <c r="AL6" s="120"/>
-      <c r="AM6" s="120"/>
-      <c r="AN6" s="120"/>
-      <c r="AO6" s="120"/>
-      <c r="AP6" s="121"/>
-      <c r="AQ6" s="122" t="s">
+      <c r="AJ6" s="127"/>
+      <c r="AK6" s="127"/>
+      <c r="AL6" s="127"/>
+      <c r="AM6" s="127"/>
+      <c r="AN6" s="127"/>
+      <c r="AO6" s="127"/>
+      <c r="AP6" s="128"/>
+      <c r="AQ6" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="AR6" s="120"/>
-      <c r="AS6" s="120"/>
-      <c r="AT6" s="120"/>
-      <c r="AU6" s="120"/>
-      <c r="AV6" s="120"/>
-      <c r="AW6" s="120"/>
-      <c r="AX6" s="121"/>
-      <c r="AY6" s="122" t="s">
+      <c r="AR6" s="127"/>
+      <c r="AS6" s="127"/>
+      <c r="AT6" s="127"/>
+      <c r="AU6" s="127"/>
+      <c r="AV6" s="127"/>
+      <c r="AW6" s="127"/>
+      <c r="AX6" s="128"/>
+      <c r="AY6" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="AZ6" s="120"/>
-      <c r="BA6" s="120"/>
-      <c r="BB6" s="120"/>
-      <c r="BC6" s="120"/>
-      <c r="BD6" s="120"/>
-      <c r="BE6" s="120"/>
-      <c r="BF6" s="121"/>
-      <c r="BG6" s="122" t="s">
+      <c r="AZ6" s="127"/>
+      <c r="BA6" s="127"/>
+      <c r="BB6" s="127"/>
+      <c r="BC6" s="127"/>
+      <c r="BD6" s="127"/>
+      <c r="BE6" s="127"/>
+      <c r="BF6" s="128"/>
+      <c r="BG6" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="BH6" s="120"/>
-      <c r="BI6" s="120"/>
-      <c r="BJ6" s="120"/>
-      <c r="BK6" s="120"/>
-      <c r="BL6" s="120"/>
-      <c r="BM6" s="120"/>
-      <c r="BN6" s="121"/>
-      <c r="BO6" s="111" t="s">
+      <c r="BH6" s="127"/>
+      <c r="BI6" s="127"/>
+      <c r="BJ6" s="127"/>
+      <c r="BK6" s="127"/>
+      <c r="BL6" s="127"/>
+      <c r="BM6" s="127"/>
+      <c r="BN6" s="128"/>
+      <c r="BO6" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="BP6" s="112"/>
-      <c r="BQ6" s="112"/>
-      <c r="BR6" s="112"/>
-      <c r="BS6" s="112"/>
-      <c r="BT6" s="112"/>
-      <c r="BU6" s="112"/>
-      <c r="BV6" s="113"/>
-      <c r="BW6" s="119" t="s">
+      <c r="BP6" s="119"/>
+      <c r="BQ6" s="119"/>
+      <c r="BR6" s="119"/>
+      <c r="BS6" s="119"/>
+      <c r="BT6" s="119"/>
+      <c r="BU6" s="119"/>
+      <c r="BV6" s="120"/>
+      <c r="BW6" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="BX6" s="120"/>
-      <c r="BY6" s="120"/>
-      <c r="BZ6" s="120"/>
-      <c r="CA6" s="120"/>
-      <c r="CB6" s="120"/>
-      <c r="CC6" s="120"/>
-      <c r="CD6" s="121"/>
-      <c r="CE6" s="122" t="s">
+      <c r="BX6" s="127"/>
+      <c r="BY6" s="127"/>
+      <c r="BZ6" s="127"/>
+      <c r="CA6" s="127"/>
+      <c r="CB6" s="127"/>
+      <c r="CC6" s="127"/>
+      <c r="CD6" s="128"/>
+      <c r="CE6" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="CF6" s="120"/>
-      <c r="CG6" s="120"/>
-      <c r="CH6" s="120"/>
-      <c r="CI6" s="120"/>
-      <c r="CJ6" s="120"/>
-      <c r="CK6" s="120"/>
-      <c r="CL6" s="121"/>
-      <c r="CM6" s="122" t="s">
+      <c r="CF6" s="127"/>
+      <c r="CG6" s="127"/>
+      <c r="CH6" s="127"/>
+      <c r="CI6" s="127"/>
+      <c r="CJ6" s="127"/>
+      <c r="CK6" s="127"/>
+      <c r="CL6" s="128"/>
+      <c r="CM6" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="CN6" s="120"/>
-      <c r="CO6" s="120"/>
-      <c r="CP6" s="120"/>
-      <c r="CQ6" s="120"/>
-      <c r="CR6" s="120"/>
-      <c r="CS6" s="120"/>
-      <c r="CT6" s="121"/>
-      <c r="CU6" s="122" t="s">
+      <c r="CN6" s="127"/>
+      <c r="CO6" s="127"/>
+      <c r="CP6" s="127"/>
+      <c r="CQ6" s="127"/>
+      <c r="CR6" s="127"/>
+      <c r="CS6" s="127"/>
+      <c r="CT6" s="128"/>
+      <c r="CU6" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="CV6" s="120"/>
-      <c r="CW6" s="120"/>
-      <c r="CX6" s="120"/>
-      <c r="CY6" s="120"/>
-      <c r="CZ6" s="120"/>
-      <c r="DA6" s="120"/>
-      <c r="DB6" s="121"/>
-      <c r="DC6" s="111" t="s">
+      <c r="CV6" s="127"/>
+      <c r="CW6" s="127"/>
+      <c r="CX6" s="127"/>
+      <c r="CY6" s="127"/>
+      <c r="CZ6" s="127"/>
+      <c r="DA6" s="127"/>
+      <c r="DB6" s="128"/>
+      <c r="DC6" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="DD6" s="112"/>
-      <c r="DE6" s="112"/>
-      <c r="DF6" s="112"/>
-      <c r="DG6" s="112"/>
-      <c r="DH6" s="112"/>
-      <c r="DI6" s="112"/>
-      <c r="DJ6" s="113"/>
-      <c r="DK6" s="119" t="s">
+      <c r="DD6" s="119"/>
+      <c r="DE6" s="119"/>
+      <c r="DF6" s="119"/>
+      <c r="DG6" s="119"/>
+      <c r="DH6" s="119"/>
+      <c r="DI6" s="119"/>
+      <c r="DJ6" s="120"/>
+      <c r="DK6" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="DL6" s="120"/>
-      <c r="DM6" s="120"/>
-      <c r="DN6" s="120"/>
-      <c r="DO6" s="120"/>
-      <c r="DP6" s="120"/>
-      <c r="DQ6" s="120"/>
-      <c r="DR6" s="121"/>
-      <c r="DS6" s="122" t="s">
+      <c r="DL6" s="127"/>
+      <c r="DM6" s="127"/>
+      <c r="DN6" s="127"/>
+      <c r="DO6" s="127"/>
+      <c r="DP6" s="127"/>
+      <c r="DQ6" s="127"/>
+      <c r="DR6" s="128"/>
+      <c r="DS6" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="DT6" s="120"/>
-      <c r="DU6" s="120"/>
-      <c r="DV6" s="120"/>
-      <c r="DW6" s="120"/>
-      <c r="DX6" s="120"/>
-      <c r="DY6" s="120"/>
-      <c r="DZ6" s="121"/>
-      <c r="EA6" s="122" t="s">
+      <c r="DT6" s="127"/>
+      <c r="DU6" s="127"/>
+      <c r="DV6" s="127"/>
+      <c r="DW6" s="127"/>
+      <c r="DX6" s="127"/>
+      <c r="DY6" s="127"/>
+      <c r="DZ6" s="128"/>
+      <c r="EA6" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="EB6" s="120"/>
-      <c r="EC6" s="120"/>
-      <c r="ED6" s="120"/>
-      <c r="EE6" s="120"/>
-      <c r="EF6" s="120"/>
-      <c r="EG6" s="120"/>
-      <c r="EH6" s="121"/>
-      <c r="EI6" s="122" t="s">
+      <c r="EB6" s="127"/>
+      <c r="EC6" s="127"/>
+      <c r="ED6" s="127"/>
+      <c r="EE6" s="127"/>
+      <c r="EF6" s="127"/>
+      <c r="EG6" s="127"/>
+      <c r="EH6" s="128"/>
+      <c r="EI6" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="EJ6" s="120"/>
-      <c r="EK6" s="120"/>
-      <c r="EL6" s="120"/>
-      <c r="EM6" s="120"/>
-      <c r="EN6" s="120"/>
-      <c r="EO6" s="120"/>
-      <c r="EP6" s="121"/>
-      <c r="EQ6" s="111" t="s">
+      <c r="EJ6" s="127"/>
+      <c r="EK6" s="127"/>
+      <c r="EL6" s="127"/>
+      <c r="EM6" s="127"/>
+      <c r="EN6" s="127"/>
+      <c r="EO6" s="127"/>
+      <c r="EP6" s="128"/>
+      <c r="EQ6" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="ER6" s="112"/>
-      <c r="ES6" s="112"/>
-      <c r="ET6" s="112"/>
-      <c r="EU6" s="112"/>
-      <c r="EV6" s="112"/>
-      <c r="EW6" s="112"/>
-      <c r="EX6" s="113"/>
-      <c r="EY6" s="119" t="s">
+      <c r="ER6" s="119"/>
+      <c r="ES6" s="119"/>
+      <c r="ET6" s="119"/>
+      <c r="EU6" s="119"/>
+      <c r="EV6" s="119"/>
+      <c r="EW6" s="119"/>
+      <c r="EX6" s="120"/>
+      <c r="EY6" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="EZ6" s="120"/>
-      <c r="FA6" s="120"/>
-      <c r="FB6" s="120"/>
-      <c r="FC6" s="120"/>
-      <c r="FD6" s="120"/>
-      <c r="FE6" s="120"/>
-      <c r="FF6" s="121"/>
+      <c r="EZ6" s="127"/>
+      <c r="FA6" s="127"/>
+      <c r="FB6" s="127"/>
+      <c r="FC6" s="127"/>
+      <c r="FD6" s="127"/>
+      <c r="FE6" s="127"/>
+      <c r="FF6" s="128"/>
     </row>
     <row r="7" spans="1:162" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -2562,14 +2617,14 @@
       <c r="EF8" s="5"/>
       <c r="EG8" s="5"/>
       <c r="EH8" s="9"/>
-      <c r="EI8" s="8"/>
-      <c r="EJ8" s="5"/>
-      <c r="EK8" s="5"/>
-      <c r="EL8" s="5"/>
-      <c r="EM8" s="5"/>
-      <c r="EN8" s="5"/>
-      <c r="EO8" s="5"/>
-      <c r="EP8" s="9"/>
+      <c r="EI8" s="107"/>
+      <c r="EJ8" s="108"/>
+      <c r="EK8" s="108"/>
+      <c r="EL8" s="108"/>
+      <c r="EM8" s="108"/>
+      <c r="EN8" s="108"/>
+      <c r="EO8" s="108"/>
+      <c r="EP8" s="109"/>
       <c r="EQ8" s="90"/>
       <c r="ER8" s="91"/>
       <c r="ES8" s="91"/>
@@ -2730,14 +2785,14 @@
       <c r="EF9" s="5"/>
       <c r="EG9" s="5"/>
       <c r="EH9" s="9"/>
-      <c r="EI9" s="8"/>
-      <c r="EJ9" s="5"/>
-      <c r="EK9" s="5"/>
-      <c r="EL9" s="5"/>
-      <c r="EM9" s="5"/>
-      <c r="EN9" s="5"/>
-      <c r="EO9" s="5"/>
-      <c r="EP9" s="9"/>
+      <c r="EI9" s="107"/>
+      <c r="EJ9" s="108"/>
+      <c r="EK9" s="108"/>
+      <c r="EL9" s="108"/>
+      <c r="EM9" s="108"/>
+      <c r="EN9" s="108"/>
+      <c r="EO9" s="108"/>
+      <c r="EP9" s="109"/>
       <c r="EQ9" s="90"/>
       <c r="ER9" s="91"/>
       <c r="ES9" s="91"/>
@@ -2904,14 +2959,14 @@
       <c r="EF10" s="5"/>
       <c r="EG10" s="5"/>
       <c r="EH10" s="9"/>
-      <c r="EI10" s="8"/>
-      <c r="EJ10" s="5"/>
-      <c r="EK10" s="5"/>
-      <c r="EL10" s="5"/>
-      <c r="EM10" s="5"/>
-      <c r="EN10" s="5"/>
-      <c r="EO10" s="5"/>
-      <c r="EP10" s="9"/>
+      <c r="EI10" s="107"/>
+      <c r="EJ10" s="108"/>
+      <c r="EK10" s="108"/>
+      <c r="EL10" s="108"/>
+      <c r="EM10" s="108"/>
+      <c r="EN10" s="108"/>
+      <c r="EO10" s="108"/>
+      <c r="EP10" s="109"/>
       <c r="EQ10" s="93"/>
       <c r="ER10" s="76"/>
       <c r="ES10" s="76"/>
@@ -3071,14 +3126,14 @@
       <c r="EF11" s="5"/>
       <c r="EG11" s="5"/>
       <c r="EH11" s="9"/>
-      <c r="EI11" s="8"/>
-      <c r="EJ11" s="5"/>
-      <c r="EK11" s="5"/>
-      <c r="EL11" s="5"/>
-      <c r="EM11" s="5"/>
-      <c r="EN11" s="5"/>
-      <c r="EO11" s="5"/>
-      <c r="EP11" s="9"/>
+      <c r="EI11" s="107"/>
+      <c r="EJ11" s="108"/>
+      <c r="EK11" s="108"/>
+      <c r="EL11" s="108"/>
+      <c r="EM11" s="108"/>
+      <c r="EN11" s="108"/>
+      <c r="EO11" s="108"/>
+      <c r="EP11" s="109"/>
       <c r="EQ11" s="93"/>
       <c r="ER11" s="76"/>
       <c r="ES11" s="76"/>
@@ -3243,14 +3298,14 @@
       <c r="EF12" s="5"/>
       <c r="EG12" s="5"/>
       <c r="EH12" s="9"/>
-      <c r="EI12" s="8"/>
-      <c r="EJ12" s="5"/>
-      <c r="EK12" s="5"/>
-      <c r="EL12" s="5"/>
-      <c r="EM12" s="5"/>
-      <c r="EN12" s="5"/>
-      <c r="EO12" s="5"/>
-      <c r="EP12" s="9"/>
+      <c r="EI12" s="107"/>
+      <c r="EJ12" s="108"/>
+      <c r="EK12" s="108"/>
+      <c r="EL12" s="108"/>
+      <c r="EM12" s="108"/>
+      <c r="EN12" s="108"/>
+      <c r="EO12" s="108"/>
+      <c r="EP12" s="109"/>
       <c r="EQ12" s="93"/>
       <c r="ER12" s="76"/>
       <c r="ES12" s="76"/>
@@ -3423,14 +3478,14 @@
       <c r="EF13" s="5"/>
       <c r="EG13" s="5"/>
       <c r="EH13" s="9"/>
-      <c r="EI13" s="8"/>
-      <c r="EJ13" s="5"/>
-      <c r="EK13" s="5"/>
-      <c r="EL13" s="5"/>
-      <c r="EM13" s="5"/>
-      <c r="EN13" s="5"/>
-      <c r="EO13" s="5"/>
-      <c r="EP13" s="9"/>
+      <c r="EI13" s="107"/>
+      <c r="EJ13" s="108"/>
+      <c r="EK13" s="108"/>
+      <c r="EL13" s="108"/>
+      <c r="EM13" s="108"/>
+      <c r="EN13" s="108"/>
+      <c r="EO13" s="108"/>
+      <c r="EP13" s="109"/>
       <c r="EQ13" s="93"/>
       <c r="ER13" s="76"/>
       <c r="ES13" s="76"/>
@@ -3591,14 +3646,14 @@
       <c r="EF14" s="5"/>
       <c r="EG14" s="5"/>
       <c r="EH14" s="9"/>
-      <c r="EI14" s="8"/>
-      <c r="EJ14" s="5"/>
-      <c r="EK14" s="5"/>
-      <c r="EL14" s="5"/>
-      <c r="EM14" s="5"/>
-      <c r="EN14" s="5"/>
-      <c r="EO14" s="5"/>
-      <c r="EP14" s="9"/>
+      <c r="EI14" s="107"/>
+      <c r="EJ14" s="108"/>
+      <c r="EK14" s="108"/>
+      <c r="EL14" s="108"/>
+      <c r="EM14" s="108"/>
+      <c r="EN14" s="108"/>
+      <c r="EO14" s="108"/>
+      <c r="EP14" s="109"/>
       <c r="EQ14" s="93"/>
       <c r="ER14" s="76"/>
       <c r="ES14" s="76"/>
@@ -3771,14 +3826,14 @@
       <c r="EF15" s="5"/>
       <c r="EG15" s="5"/>
       <c r="EH15" s="9"/>
-      <c r="EI15" s="8"/>
-      <c r="EJ15" s="5"/>
-      <c r="EK15" s="5"/>
-      <c r="EL15" s="5"/>
-      <c r="EM15" s="5"/>
-      <c r="EN15" s="5"/>
-      <c r="EO15" s="5"/>
-      <c r="EP15" s="9"/>
+      <c r="EI15" s="107"/>
+      <c r="EJ15" s="108"/>
+      <c r="EK15" s="108"/>
+      <c r="EL15" s="108"/>
+      <c r="EM15" s="108"/>
+      <c r="EN15" s="108"/>
+      <c r="EO15" s="108"/>
+      <c r="EP15" s="109"/>
       <c r="EQ15" s="93"/>
       <c r="ER15" s="76"/>
       <c r="ES15" s="76"/>
@@ -3942,14 +3997,14 @@
       <c r="EF16" s="5"/>
       <c r="EG16" s="5"/>
       <c r="EH16" s="9"/>
-      <c r="EI16" s="8"/>
-      <c r="EJ16" s="5"/>
-      <c r="EK16" s="5"/>
-      <c r="EL16" s="5"/>
-      <c r="EM16" s="5"/>
-      <c r="EN16" s="5"/>
-      <c r="EO16" s="5"/>
-      <c r="EP16" s="9"/>
+      <c r="EI16" s="107"/>
+      <c r="EJ16" s="108"/>
+      <c r="EK16" s="108"/>
+      <c r="EL16" s="108"/>
+      <c r="EM16" s="108"/>
+      <c r="EN16" s="108"/>
+      <c r="EO16" s="108"/>
+      <c r="EP16" s="109"/>
       <c r="EQ16" s="93"/>
       <c r="ER16" s="76"/>
       <c r="ES16" s="76"/>
@@ -4107,14 +4162,14 @@
       <c r="EF17" s="5"/>
       <c r="EG17" s="5"/>
       <c r="EH17" s="9"/>
-      <c r="EI17" s="8"/>
-      <c r="EJ17" s="5"/>
-      <c r="EK17" s="5"/>
-      <c r="EL17" s="5"/>
-      <c r="EM17" s="5"/>
-      <c r="EN17" s="5"/>
-      <c r="EO17" s="5"/>
-      <c r="EP17" s="9"/>
+      <c r="EI17" s="107"/>
+      <c r="EJ17" s="108"/>
+      <c r="EK17" s="108"/>
+      <c r="EL17" s="108"/>
+      <c r="EM17" s="108"/>
+      <c r="EN17" s="108"/>
+      <c r="EO17" s="108"/>
+      <c r="EP17" s="109"/>
       <c r="EQ17" s="95"/>
       <c r="ER17" s="76"/>
       <c r="ES17" s="76"/>
@@ -4273,14 +4328,14 @@
       <c r="EF18" s="5"/>
       <c r="EG18" s="5"/>
       <c r="EH18" s="9"/>
-      <c r="EI18" s="8"/>
-      <c r="EJ18" s="5"/>
-      <c r="EK18" s="5"/>
-      <c r="EL18" s="5"/>
-      <c r="EM18" s="5"/>
-      <c r="EN18" s="5"/>
-      <c r="EO18" s="5"/>
-      <c r="EP18" s="9"/>
+      <c r="EI18" s="107"/>
+      <c r="EJ18" s="108"/>
+      <c r="EK18" s="108"/>
+      <c r="EL18" s="108"/>
+      <c r="EM18" s="108"/>
+      <c r="EN18" s="108"/>
+      <c r="EO18" s="108"/>
+      <c r="EP18" s="109"/>
       <c r="EQ18" s="95"/>
       <c r="ER18" s="76"/>
       <c r="ES18" s="76"/>
@@ -4441,14 +4496,14 @@
       <c r="EF19" s="5"/>
       <c r="EG19" s="5"/>
       <c r="EH19" s="9"/>
-      <c r="EI19" s="8"/>
-      <c r="EJ19" s="5"/>
-      <c r="EK19" s="5"/>
-      <c r="EL19" s="5"/>
-      <c r="EM19" s="5"/>
-      <c r="EN19" s="5"/>
-      <c r="EO19" s="5"/>
-      <c r="EP19" s="9"/>
+      <c r="EI19" s="107"/>
+      <c r="EJ19" s="108"/>
+      <c r="EK19" s="108"/>
+      <c r="EL19" s="108"/>
+      <c r="EM19" s="108"/>
+      <c r="EN19" s="108"/>
+      <c r="EO19" s="108"/>
+      <c r="EP19" s="109"/>
       <c r="EQ19" s="95"/>
       <c r="ER19" s="76"/>
       <c r="ES19" s="76"/>
@@ -4623,14 +4678,14 @@
       <c r="EF20" s="5"/>
       <c r="EG20" s="5"/>
       <c r="EH20" s="9"/>
-      <c r="EI20" s="8"/>
-      <c r="EJ20" s="5"/>
-      <c r="EK20" s="5"/>
-      <c r="EL20" s="5"/>
-      <c r="EM20" s="5"/>
-      <c r="EN20" s="5"/>
-      <c r="EO20" s="5"/>
-      <c r="EP20" s="9"/>
+      <c r="EI20" s="107"/>
+      <c r="EJ20" s="108"/>
+      <c r="EK20" s="108"/>
+      <c r="EL20" s="108"/>
+      <c r="EM20" s="108"/>
+      <c r="EN20" s="108"/>
+      <c r="EO20" s="108"/>
+      <c r="EP20" s="109"/>
       <c r="EQ20" s="95"/>
       <c r="ER20" s="76"/>
       <c r="ES20" s="76"/>
@@ -4791,14 +4846,14 @@
       <c r="EF21" s="5"/>
       <c r="EG21" s="5"/>
       <c r="EH21" s="9"/>
-      <c r="EI21" s="8"/>
-      <c r="EJ21" s="5"/>
-      <c r="EK21" s="5"/>
-      <c r="EL21" s="5"/>
-      <c r="EM21" s="5"/>
-      <c r="EN21" s="5"/>
-      <c r="EO21" s="5"/>
-      <c r="EP21" s="9"/>
+      <c r="EI21" s="107"/>
+      <c r="EJ21" s="108"/>
+      <c r="EK21" s="108"/>
+      <c r="EL21" s="108"/>
+      <c r="EM21" s="108"/>
+      <c r="EN21" s="108"/>
+      <c r="EO21" s="108"/>
+      <c r="EP21" s="109"/>
       <c r="EQ21" s="95"/>
       <c r="ER21" s="76"/>
       <c r="ES21" s="76"/>
@@ -4961,14 +5016,14 @@
       <c r="EF22" s="5"/>
       <c r="EG22" s="5"/>
       <c r="EH22" s="9"/>
-      <c r="EI22" s="8"/>
-      <c r="EJ22" s="5"/>
-      <c r="EK22" s="5"/>
-      <c r="EL22" s="5"/>
-      <c r="EM22" s="5"/>
-      <c r="EN22" s="5"/>
-      <c r="EO22" s="5"/>
-      <c r="EP22" s="9"/>
+      <c r="EI22" s="107"/>
+      <c r="EJ22" s="108"/>
+      <c r="EK22" s="108"/>
+      <c r="EL22" s="108"/>
+      <c r="EM22" s="108"/>
+      <c r="EN22" s="108"/>
+      <c r="EO22" s="108"/>
+      <c r="EP22" s="109"/>
       <c r="EQ22" s="95"/>
       <c r="ER22" s="76"/>
       <c r="ES22" s="76"/>
@@ -5134,14 +5189,14 @@
       <c r="EF23" s="5"/>
       <c r="EG23" s="5"/>
       <c r="EH23" s="9"/>
-      <c r="EI23" s="8"/>
-      <c r="EJ23" s="5"/>
-      <c r="EK23" s="5"/>
-      <c r="EL23" s="5"/>
-      <c r="EM23" s="5"/>
-      <c r="EN23" s="5"/>
-      <c r="EO23" s="5"/>
-      <c r="EP23" s="9"/>
+      <c r="EI23" s="107"/>
+      <c r="EJ23" s="108"/>
+      <c r="EK23" s="108"/>
+      <c r="EL23" s="108"/>
+      <c r="EM23" s="108"/>
+      <c r="EN23" s="108"/>
+      <c r="EO23" s="108"/>
+      <c r="EP23" s="109"/>
       <c r="EQ23" s="95"/>
       <c r="ER23" s="76"/>
       <c r="ES23" s="76"/>
@@ -5306,14 +5361,14 @@
       <c r="EF24" s="5"/>
       <c r="EG24" s="5"/>
       <c r="EH24" s="9"/>
-      <c r="EI24" s="8"/>
-      <c r="EJ24" s="5"/>
-      <c r="EK24" s="5"/>
-      <c r="EL24" s="5"/>
-      <c r="EM24" s="5"/>
-      <c r="EN24" s="5"/>
-      <c r="EO24" s="5"/>
-      <c r="EP24" s="9"/>
+      <c r="EI24" s="107"/>
+      <c r="EJ24" s="108"/>
+      <c r="EK24" s="108"/>
+      <c r="EL24" s="108"/>
+      <c r="EM24" s="108"/>
+      <c r="EN24" s="108"/>
+      <c r="EO24" s="108"/>
+      <c r="EP24" s="109"/>
       <c r="EQ24" s="95"/>
       <c r="ER24" s="76"/>
       <c r="ES24" s="76"/>
@@ -5478,14 +5533,14 @@
       <c r="EF25" s="5"/>
       <c r="EG25" s="5"/>
       <c r="EH25" s="9"/>
-      <c r="EI25" s="8"/>
-      <c r="EJ25" s="5"/>
-      <c r="EK25" s="5"/>
-      <c r="EL25" s="5"/>
-      <c r="EM25" s="5"/>
-      <c r="EN25" s="5"/>
-      <c r="EO25" s="5"/>
-      <c r="EP25" s="9"/>
+      <c r="EI25" s="107"/>
+      <c r="EJ25" s="108"/>
+      <c r="EK25" s="108"/>
+      <c r="EL25" s="108"/>
+      <c r="EM25" s="108"/>
+      <c r="EN25" s="108"/>
+      <c r="EO25" s="108"/>
+      <c r="EP25" s="109"/>
       <c r="EQ25" s="95"/>
       <c r="ER25" s="76"/>
       <c r="ES25" s="76"/>
@@ -5647,14 +5702,14 @@
       <c r="EF26" s="5"/>
       <c r="EG26" s="5"/>
       <c r="EH26" s="9"/>
-      <c r="EI26" s="8"/>
-      <c r="EJ26" s="5"/>
-      <c r="EK26" s="5"/>
-      <c r="EL26" s="5"/>
-      <c r="EM26" s="5"/>
-      <c r="EN26" s="5"/>
-      <c r="EO26" s="5"/>
-      <c r="EP26" s="9"/>
+      <c r="EI26" s="107"/>
+      <c r="EJ26" s="108"/>
+      <c r="EK26" s="108"/>
+      <c r="EL26" s="108"/>
+      <c r="EM26" s="108"/>
+      <c r="EN26" s="108"/>
+      <c r="EO26" s="108"/>
+      <c r="EP26" s="109"/>
       <c r="EQ26" s="95"/>
       <c r="ER26" s="76"/>
       <c r="ES26" s="76"/>
@@ -5817,14 +5872,14 @@
       <c r="EF27" s="5"/>
       <c r="EG27" s="5"/>
       <c r="EH27" s="9"/>
-      <c r="EI27" s="8"/>
-      <c r="EJ27" s="5"/>
-      <c r="EK27" s="5"/>
-      <c r="EL27" s="5"/>
-      <c r="EM27" s="5"/>
-      <c r="EN27" s="5"/>
-      <c r="EO27" s="5"/>
-      <c r="EP27" s="9"/>
+      <c r="EI27" s="107"/>
+      <c r="EJ27" s="108"/>
+      <c r="EK27" s="108"/>
+      <c r="EL27" s="108"/>
+      <c r="EM27" s="108"/>
+      <c r="EN27" s="108"/>
+      <c r="EO27" s="108"/>
+      <c r="EP27" s="109"/>
       <c r="EQ27" s="95"/>
       <c r="ER27" s="76"/>
       <c r="ES27" s="76"/>
@@ -5988,14 +6043,14 @@
       <c r="EF28" s="5"/>
       <c r="EG28" s="5"/>
       <c r="EH28" s="9"/>
-      <c r="EI28" s="8"/>
-      <c r="EJ28" s="5"/>
-      <c r="EK28" s="5"/>
-      <c r="EL28" s="5"/>
-      <c r="EM28" s="5"/>
-      <c r="EN28" s="5"/>
-      <c r="EO28" s="5"/>
-      <c r="EP28" s="9"/>
+      <c r="EI28" s="107"/>
+      <c r="EJ28" s="108"/>
+      <c r="EK28" s="108"/>
+      <c r="EL28" s="108"/>
+      <c r="EM28" s="108"/>
+      <c r="EN28" s="108"/>
+      <c r="EO28" s="108"/>
+      <c r="EP28" s="109"/>
       <c r="EQ28" s="95"/>
       <c r="ER28" s="76"/>
       <c r="ES28" s="76"/>
@@ -6158,14 +6213,14 @@
       <c r="EF29" s="5"/>
       <c r="EG29" s="5"/>
       <c r="EH29" s="9"/>
-      <c r="EI29" s="8"/>
-      <c r="EJ29" s="5"/>
-      <c r="EK29" s="5"/>
-      <c r="EL29" s="5"/>
-      <c r="EM29" s="5"/>
-      <c r="EN29" s="5"/>
-      <c r="EO29" s="5"/>
-      <c r="EP29" s="9"/>
+      <c r="EI29" s="107"/>
+      <c r="EJ29" s="108"/>
+      <c r="EK29" s="108"/>
+      <c r="EL29" s="108"/>
+      <c r="EM29" s="108"/>
+      <c r="EN29" s="108"/>
+      <c r="EO29" s="108"/>
+      <c r="EP29" s="109"/>
       <c r="EQ29" s="95"/>
       <c r="ER29" s="76"/>
       <c r="ES29" s="76"/>
@@ -6362,14 +6417,14 @@
       <c r="EF30" s="5"/>
       <c r="EG30" s="5"/>
       <c r="EH30" s="9"/>
-      <c r="EI30" s="8"/>
-      <c r="EJ30" s="5"/>
-      <c r="EK30" s="5"/>
-      <c r="EL30" s="5"/>
-      <c r="EM30" s="5"/>
-      <c r="EN30" s="5"/>
-      <c r="EO30" s="5"/>
-      <c r="EP30" s="9"/>
+      <c r="EI30" s="107"/>
+      <c r="EJ30" s="108"/>
+      <c r="EK30" s="108"/>
+      <c r="EL30" s="108"/>
+      <c r="EM30" s="108"/>
+      <c r="EN30" s="108"/>
+      <c r="EO30" s="108"/>
+      <c r="EP30" s="109"/>
       <c r="EQ30" s="95"/>
       <c r="ER30" s="76"/>
       <c r="ES30" s="76"/>
@@ -6530,14 +6585,14 @@
       <c r="EF31" s="5"/>
       <c r="EG31" s="5"/>
       <c r="EH31" s="9"/>
-      <c r="EI31" s="8"/>
-      <c r="EJ31" s="5"/>
-      <c r="EK31" s="5"/>
-      <c r="EL31" s="5"/>
-      <c r="EM31" s="5"/>
-      <c r="EN31" s="5"/>
-      <c r="EO31" s="5"/>
-      <c r="EP31" s="9"/>
+      <c r="EI31" s="107"/>
+      <c r="EJ31" s="108"/>
+      <c r="EK31" s="108"/>
+      <c r="EL31" s="108"/>
+      <c r="EM31" s="108"/>
+      <c r="EN31" s="108"/>
+      <c r="EO31" s="108"/>
+      <c r="EP31" s="109"/>
       <c r="EQ31" s="95"/>
       <c r="ER31" s="76"/>
       <c r="ES31" s="76"/>
@@ -6710,14 +6765,14 @@
       <c r="EF32" s="5"/>
       <c r="EG32" s="5"/>
       <c r="EH32" s="9"/>
-      <c r="EI32" s="8"/>
-      <c r="EJ32" s="5"/>
-      <c r="EK32" s="5"/>
-      <c r="EL32" s="5"/>
-      <c r="EM32" s="5"/>
-      <c r="EN32" s="5"/>
-      <c r="EO32" s="5"/>
-      <c r="EP32" s="9"/>
+      <c r="EI32" s="107"/>
+      <c r="EJ32" s="108"/>
+      <c r="EK32" s="108"/>
+      <c r="EL32" s="108"/>
+      <c r="EM32" s="108"/>
+      <c r="EN32" s="108"/>
+      <c r="EO32" s="108"/>
+      <c r="EP32" s="109"/>
       <c r="EQ32" s="95"/>
       <c r="ER32" s="76"/>
       <c r="ES32" s="76"/>
@@ -6878,14 +6933,14 @@
       <c r="EF33" s="5"/>
       <c r="EG33" s="5"/>
       <c r="EH33" s="9"/>
-      <c r="EI33" s="8"/>
-      <c r="EJ33" s="5"/>
-      <c r="EK33" s="5"/>
-      <c r="EL33" s="5"/>
-      <c r="EM33" s="5"/>
-      <c r="EN33" s="5"/>
-      <c r="EO33" s="5"/>
-      <c r="EP33" s="9"/>
+      <c r="EI33" s="107"/>
+      <c r="EJ33" s="108"/>
+      <c r="EK33" s="108"/>
+      <c r="EL33" s="108"/>
+      <c r="EM33" s="108"/>
+      <c r="EN33" s="108"/>
+      <c r="EO33" s="108"/>
+      <c r="EP33" s="109"/>
       <c r="EQ33" s="95"/>
       <c r="ER33" s="76"/>
       <c r="ES33" s="76"/>
@@ -7053,14 +7108,14 @@
       <c r="EF34" s="5"/>
       <c r="EG34" s="5"/>
       <c r="EH34" s="9"/>
-      <c r="EI34" s="8"/>
-      <c r="EJ34" s="5"/>
-      <c r="EK34" s="5"/>
-      <c r="EL34" s="5"/>
-      <c r="EM34" s="5"/>
-      <c r="EN34" s="5"/>
-      <c r="EO34" s="5"/>
-      <c r="EP34" s="9"/>
+      <c r="EI34" s="107"/>
+      <c r="EJ34" s="108"/>
+      <c r="EK34" s="108"/>
+      <c r="EL34" s="108"/>
+      <c r="EM34" s="108"/>
+      <c r="EN34" s="108"/>
+      <c r="EO34" s="108"/>
+      <c r="EP34" s="109"/>
       <c r="EQ34" s="95"/>
       <c r="ER34" s="76"/>
       <c r="ES34" s="76"/>
@@ -7220,14 +7275,14 @@
       <c r="EF35" s="5"/>
       <c r="EG35" s="5"/>
       <c r="EH35" s="9"/>
-      <c r="EI35" s="8"/>
-      <c r="EJ35" s="5"/>
-      <c r="EK35" s="5"/>
-      <c r="EL35" s="5"/>
-      <c r="EM35" s="5"/>
-      <c r="EN35" s="5"/>
-      <c r="EO35" s="5"/>
-      <c r="EP35" s="9"/>
+      <c r="EI35" s="107"/>
+      <c r="EJ35" s="108"/>
+      <c r="EK35" s="108"/>
+      <c r="EL35" s="108"/>
+      <c r="EM35" s="108"/>
+      <c r="EN35" s="108"/>
+      <c r="EO35" s="108"/>
+      <c r="EP35" s="109"/>
       <c r="EQ35" s="90"/>
       <c r="ER35" s="91"/>
       <c r="ES35" s="91"/>
@@ -7408,14 +7463,14 @@
       <c r="EF36" s="5"/>
       <c r="EG36" s="5"/>
       <c r="EH36" s="9"/>
-      <c r="EI36" s="8"/>
-      <c r="EJ36" s="5"/>
-      <c r="EK36" s="5"/>
-      <c r="EL36" s="5"/>
-      <c r="EM36" s="5"/>
-      <c r="EN36" s="5"/>
-      <c r="EO36" s="5"/>
-      <c r="EP36" s="9"/>
+      <c r="EI36" s="107"/>
+      <c r="EJ36" s="108"/>
+      <c r="EK36" s="108"/>
+      <c r="EL36" s="108"/>
+      <c r="EM36" s="108"/>
+      <c r="EN36" s="108"/>
+      <c r="EO36" s="108"/>
+      <c r="EP36" s="109"/>
       <c r="EQ36" s="90"/>
       <c r="ER36" s="91"/>
       <c r="ES36" s="91"/>
@@ -7598,14 +7653,14 @@
       <c r="EF37" s="5"/>
       <c r="EG37" s="5"/>
       <c r="EH37" s="9"/>
-      <c r="EI37" s="8"/>
-      <c r="EJ37" s="5"/>
-      <c r="EK37" s="5"/>
-      <c r="EL37" s="5"/>
-      <c r="EM37" s="5"/>
-      <c r="EN37" s="5"/>
-      <c r="EO37" s="5"/>
-      <c r="EP37" s="9"/>
+      <c r="EI37" s="107"/>
+      <c r="EJ37" s="108"/>
+      <c r="EK37" s="108"/>
+      <c r="EL37" s="108"/>
+      <c r="EM37" s="108"/>
+      <c r="EN37" s="108"/>
+      <c r="EO37" s="108"/>
+      <c r="EP37" s="109"/>
       <c r="EQ37" s="93"/>
       <c r="ER37" s="76"/>
       <c r="ES37" s="76"/>
@@ -7768,14 +7823,14 @@
       <c r="EF38" s="5"/>
       <c r="EG38" s="5"/>
       <c r="EH38" s="9"/>
-      <c r="EI38" s="8"/>
-      <c r="EJ38" s="5"/>
-      <c r="EK38" s="5"/>
-      <c r="EL38" s="5"/>
-      <c r="EM38" s="5"/>
-      <c r="EN38" s="5"/>
-      <c r="EO38" s="5"/>
-      <c r="EP38" s="9"/>
+      <c r="EI38" s="107"/>
+      <c r="EJ38" s="108"/>
+      <c r="EK38" s="108"/>
+      <c r="EL38" s="108"/>
+      <c r="EM38" s="108"/>
+      <c r="EN38" s="108"/>
+      <c r="EO38" s="108"/>
+      <c r="EP38" s="109"/>
       <c r="EQ38" s="93"/>
       <c r="ER38" s="76"/>
       <c r="ES38" s="76"/>
@@ -7936,14 +7991,14 @@
       <c r="EF39" s="5"/>
       <c r="EG39" s="5"/>
       <c r="EH39" s="9"/>
-      <c r="EI39" s="8"/>
-      <c r="EJ39" s="5"/>
-      <c r="EK39" s="5"/>
-      <c r="EL39" s="5"/>
-      <c r="EM39" s="5"/>
-      <c r="EN39" s="5"/>
-      <c r="EO39" s="5"/>
-      <c r="EP39" s="9"/>
+      <c r="EI39" s="107"/>
+      <c r="EJ39" s="108"/>
+      <c r="EK39" s="108"/>
+      <c r="EL39" s="108"/>
+      <c r="EM39" s="108"/>
+      <c r="EN39" s="108"/>
+      <c r="EO39" s="108"/>
+      <c r="EP39" s="109"/>
       <c r="EQ39" s="93"/>
       <c r="ER39" s="76"/>
       <c r="ES39" s="76"/>
@@ -8106,14 +8161,14 @@
       <c r="EF40" s="5"/>
       <c r="EG40" s="5"/>
       <c r="EH40" s="9"/>
-      <c r="EI40" s="8"/>
-      <c r="EJ40" s="5"/>
-      <c r="EK40" s="5"/>
-      <c r="EL40" s="5"/>
-      <c r="EM40" s="5"/>
-      <c r="EN40" s="5"/>
-      <c r="EO40" s="5"/>
-      <c r="EP40" s="9"/>
+      <c r="EI40" s="107"/>
+      <c r="EJ40" s="108"/>
+      <c r="EK40" s="108"/>
+      <c r="EL40" s="108"/>
+      <c r="EM40" s="108"/>
+      <c r="EN40" s="108"/>
+      <c r="EO40" s="108"/>
+      <c r="EP40" s="109"/>
       <c r="EQ40" s="93"/>
       <c r="ER40" s="76"/>
       <c r="ES40" s="76"/>
@@ -8256,9 +8311,15 @@
       <c r="DP41" s="5"/>
       <c r="DQ41" s="5"/>
       <c r="DR41" s="9"/>
-      <c r="DS41" s="74"/>
-      <c r="DT41" s="75"/>
-      <c r="DU41" s="75"/>
+      <c r="DS41" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="DT41" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="DU41" s="75" t="s">
+        <v>57</v>
+      </c>
       <c r="DV41" s="75"/>
       <c r="DW41" s="75"/>
       <c r="DX41" s="75"/>
@@ -8272,14 +8333,14 @@
       <c r="EF41" s="5"/>
       <c r="EG41" s="5"/>
       <c r="EH41" s="9"/>
-      <c r="EI41" s="8"/>
-      <c r="EJ41" s="5"/>
-      <c r="EK41" s="5"/>
-      <c r="EL41" s="5"/>
-      <c r="EM41" s="5"/>
-      <c r="EN41" s="5"/>
-      <c r="EO41" s="5"/>
-      <c r="EP41" s="9"/>
+      <c r="EI41" s="107"/>
+      <c r="EJ41" s="108"/>
+      <c r="EK41" s="108"/>
+      <c r="EL41" s="108"/>
+      <c r="EM41" s="108"/>
+      <c r="EN41" s="108"/>
+      <c r="EO41" s="108"/>
+      <c r="EP41" s="109"/>
       <c r="EQ41" s="93"/>
       <c r="ER41" s="76"/>
       <c r="ES41" s="76"/>
@@ -8427,8 +8488,12 @@
       <c r="DU42" s="75"/>
       <c r="DV42" s="75"/>
       <c r="DW42" s="75"/>
-      <c r="DX42" s="75"/>
-      <c r="DY42" s="5"/>
+      <c r="DX42" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="DY42" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="DZ42" s="9"/>
       <c r="EA42" s="8"/>
       <c r="EB42" s="5"/>
@@ -8438,14 +8503,14 @@
       <c r="EF42" s="5"/>
       <c r="EG42" s="5"/>
       <c r="EH42" s="9"/>
-      <c r="EI42" s="8"/>
-      <c r="EJ42" s="5"/>
-      <c r="EK42" s="5"/>
-      <c r="EL42" s="5"/>
-      <c r="EM42" s="5"/>
-      <c r="EN42" s="5"/>
-      <c r="EO42" s="5"/>
-      <c r="EP42" s="9"/>
+      <c r="EI42" s="107"/>
+      <c r="EJ42" s="108"/>
+      <c r="EK42" s="108"/>
+      <c r="EL42" s="108"/>
+      <c r="EM42" s="108"/>
+      <c r="EN42" s="108"/>
+      <c r="EO42" s="108"/>
+      <c r="EP42" s="109"/>
       <c r="EQ42" s="95"/>
       <c r="ER42" s="76"/>
       <c r="ES42" s="76"/>
@@ -8465,7 +8530,7 @@
     </row>
     <row r="43" spans="1:162" x14ac:dyDescent="0.2">
       <c r="A43" s="71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" s="67"/>
       <c r="C43" s="8"/>
@@ -8604,14 +8669,14 @@
       <c r="EF43" s="5"/>
       <c r="EG43" s="5"/>
       <c r="EH43" s="9"/>
-      <c r="EI43" s="8"/>
-      <c r="EJ43" s="5"/>
-      <c r="EK43" s="5"/>
-      <c r="EL43" s="5"/>
-      <c r="EM43" s="5"/>
-      <c r="EN43" s="5"/>
-      <c r="EO43" s="5"/>
-      <c r="EP43" s="9"/>
+      <c r="EI43" s="107"/>
+      <c r="EJ43" s="108"/>
+      <c r="EK43" s="108"/>
+      <c r="EL43" s="108"/>
+      <c r="EM43" s="108"/>
+      <c r="EN43" s="108"/>
+      <c r="EO43" s="108"/>
+      <c r="EP43" s="109"/>
       <c r="EQ43" s="93"/>
       <c r="ER43" s="76"/>
       <c r="ES43" s="76"/>
@@ -8760,7 +8825,9 @@
       <c r="DV44" s="5"/>
       <c r="DW44" s="5"/>
       <c r="DX44" s="5"/>
-      <c r="DY44" s="77"/>
+      <c r="DY44" s="77" t="s">
+        <v>57</v>
+      </c>
       <c r="DZ44" s="9"/>
       <c r="EA44" s="8"/>
       <c r="EB44" s="5"/>
@@ -8770,14 +8837,14 @@
       <c r="EF44" s="5"/>
       <c r="EG44" s="5"/>
       <c r="EH44" s="9"/>
-      <c r="EI44" s="8"/>
-      <c r="EJ44" s="5"/>
-      <c r="EK44" s="5"/>
-      <c r="EL44" s="5"/>
-      <c r="EM44" s="5"/>
-      <c r="EN44" s="5"/>
-      <c r="EO44" s="5"/>
-      <c r="EP44" s="9"/>
+      <c r="EI44" s="107"/>
+      <c r="EJ44" s="108"/>
+      <c r="EK44" s="108"/>
+      <c r="EL44" s="108"/>
+      <c r="EM44" s="108"/>
+      <c r="EN44" s="108"/>
+      <c r="EO44" s="108"/>
+      <c r="EP44" s="109"/>
       <c r="EQ44" s="95"/>
       <c r="ER44" s="76"/>
       <c r="ES44" s="76"/>
@@ -8923,27 +8990,49 @@
       <c r="DS45" s="27"/>
       <c r="DT45" s="23"/>
       <c r="DU45" s="23"/>
-      <c r="DV45" s="23"/>
-      <c r="DW45" s="23"/>
-      <c r="DX45" s="23"/>
-      <c r="DY45" s="23"/>
-      <c r="DZ45" s="81"/>
-      <c r="EA45" s="82"/>
+      <c r="DV45" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="DW45" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="DX45" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="DY45" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="DZ45" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="EA45" s="82" t="s">
+        <v>57</v>
+      </c>
       <c r="EB45" s="23"/>
       <c r="EC45" s="23"/>
-      <c r="ED45" s="5"/>
-      <c r="EE45" s="5"/>
-      <c r="EF45" s="23"/>
-      <c r="EG45" s="23"/>
-      <c r="EH45" s="24"/>
-      <c r="EI45" s="22"/>
-      <c r="EJ45" s="23"/>
-      <c r="EK45" s="23"/>
-      <c r="EL45" s="23"/>
-      <c r="EM45" s="23"/>
-      <c r="EN45" s="23"/>
-      <c r="EO45" s="23"/>
-      <c r="EP45" s="24"/>
+      <c r="ED45" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="EE45" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="EF45" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="EG45" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="EH45" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="EI45" s="107"/>
+      <c r="EJ45" s="108"/>
+      <c r="EK45" s="108"/>
+      <c r="EL45" s="108"/>
+      <c r="EM45" s="108"/>
+      <c r="EN45" s="108"/>
+      <c r="EO45" s="108"/>
+      <c r="EP45" s="109"/>
       <c r="EQ45" s="95"/>
       <c r="ER45" s="76"/>
       <c r="ES45" s="76"/>
@@ -9094,22 +9183,32 @@
       <c r="DX46" s="23"/>
       <c r="DY46" s="23"/>
       <c r="DZ46" s="24"/>
-      <c r="EA46" s="22"/>
-      <c r="EB46" s="86"/>
-      <c r="EC46" s="86"/>
-      <c r="ED46" s="23"/>
-      <c r="EE46" s="23"/>
+      <c r="EA46" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="EB46" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="EC46" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="ED46" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="EE46" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="EF46" s="23"/>
       <c r="EG46" s="23"/>
       <c r="EH46" s="24"/>
-      <c r="EI46" s="22"/>
-      <c r="EJ46" s="23"/>
-      <c r="EK46" s="23"/>
-      <c r="EL46" s="23"/>
-      <c r="EM46" s="23"/>
-      <c r="EN46" s="23"/>
-      <c r="EO46" s="23"/>
-      <c r="EP46" s="24"/>
+      <c r="EI46" s="107"/>
+      <c r="EJ46" s="108"/>
+      <c r="EK46" s="108"/>
+      <c r="EL46" s="108"/>
+      <c r="EM46" s="108"/>
+      <c r="EN46" s="108"/>
+      <c r="EO46" s="108"/>
+      <c r="EP46" s="109"/>
       <c r="EQ46" s="95"/>
       <c r="ER46" s="76"/>
       <c r="ES46" s="76"/>
@@ -9268,14 +9367,14 @@
       <c r="EF47" s="23"/>
       <c r="EG47" s="23"/>
       <c r="EH47" s="24"/>
-      <c r="EI47" s="27"/>
-      <c r="EJ47" s="23"/>
-      <c r="EK47" s="23"/>
-      <c r="EL47" s="23"/>
-      <c r="EM47" s="23"/>
-      <c r="EN47" s="23"/>
-      <c r="EO47" s="23"/>
-      <c r="EP47" s="24"/>
+      <c r="EI47" s="110"/>
+      <c r="EJ47" s="108"/>
+      <c r="EK47" s="108"/>
+      <c r="EL47" s="108"/>
+      <c r="EM47" s="108"/>
+      <c r="EN47" s="108"/>
+      <c r="EO47" s="108"/>
+      <c r="EP47" s="109"/>
       <c r="EQ47" s="95"/>
       <c r="ER47" s="76"/>
       <c r="ES47" s="76"/>
@@ -9434,14 +9533,14 @@
       <c r="EF48" s="77"/>
       <c r="EG48" s="77"/>
       <c r="EH48" s="81"/>
-      <c r="EI48" s="27"/>
-      <c r="EJ48" s="23"/>
-      <c r="EK48" s="23"/>
-      <c r="EL48" s="23"/>
-      <c r="EM48" s="23"/>
-      <c r="EN48" s="23"/>
-      <c r="EO48" s="23"/>
-      <c r="EP48" s="24"/>
+      <c r="EI48" s="110"/>
+      <c r="EJ48" s="108"/>
+      <c r="EK48" s="108"/>
+      <c r="EL48" s="108"/>
+      <c r="EM48" s="108"/>
+      <c r="EN48" s="108"/>
+      <c r="EO48" s="108"/>
+      <c r="EP48" s="109"/>
       <c r="EQ48" s="95"/>
       <c r="ER48" s="76"/>
       <c r="ES48" s="76"/>
@@ -9461,7 +9560,7 @@
     </row>
     <row r="49" spans="1:163" x14ac:dyDescent="0.2">
       <c r="A49" s="62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="73"/>
       <c r="C49" s="8"/>
@@ -9600,14 +9699,14 @@
       <c r="EF49" s="23"/>
       <c r="EG49" s="23"/>
       <c r="EH49" s="24"/>
-      <c r="EI49" s="80"/>
-      <c r="EJ49" s="77"/>
-      <c r="EK49" s="77"/>
-      <c r="EL49" s="77"/>
-      <c r="EM49" s="77"/>
-      <c r="EN49" s="77"/>
-      <c r="EO49" s="77"/>
-      <c r="EP49" s="81"/>
+      <c r="EI49" s="110"/>
+      <c r="EJ49" s="108"/>
+      <c r="EK49" s="108"/>
+      <c r="EL49" s="108"/>
+      <c r="EM49" s="108"/>
+      <c r="EN49" s="108"/>
+      <c r="EO49" s="108"/>
+      <c r="EP49" s="109"/>
       <c r="EQ49" s="95"/>
       <c r="ER49" s="76"/>
       <c r="ES49" s="76"/>
@@ -9764,14 +9863,14 @@
       <c r="EF50" s="23"/>
       <c r="EG50" s="23"/>
       <c r="EH50" s="24"/>
-      <c r="EI50" s="27"/>
-      <c r="EJ50" s="23"/>
-      <c r="EK50" s="23"/>
-      <c r="EL50" s="23"/>
-      <c r="EM50" s="23"/>
-      <c r="EN50" s="23"/>
-      <c r="EO50" s="23"/>
-      <c r="EP50" s="24"/>
+      <c r="EI50" s="110"/>
+      <c r="EJ50" s="108"/>
+      <c r="EK50" s="108"/>
+      <c r="EL50" s="108"/>
+      <c r="EM50" s="108"/>
+      <c r="EN50" s="108"/>
+      <c r="EO50" s="108"/>
+      <c r="EP50" s="109"/>
       <c r="EQ50" s="95"/>
       <c r="ER50" s="76"/>
       <c r="ES50" s="76"/>
@@ -9790,8 +9889,8 @@
       <c r="FF50" s="94"/>
     </row>
     <row r="51" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A51" s="114"/>
-      <c r="B51" s="123"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="130"/>
       <c r="C51" s="8"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -9928,14 +10027,14 @@
       <c r="EF51" s="23"/>
       <c r="EG51" s="23"/>
       <c r="EH51" s="24"/>
-      <c r="EI51" s="27"/>
-      <c r="EJ51" s="23"/>
-      <c r="EK51" s="23"/>
-      <c r="EL51" s="23"/>
-      <c r="EM51" s="23"/>
-      <c r="EN51" s="23"/>
-      <c r="EO51" s="23"/>
-      <c r="EP51" s="24"/>
+      <c r="EI51" s="110"/>
+      <c r="EJ51" s="108"/>
+      <c r="EK51" s="108"/>
+      <c r="EL51" s="108"/>
+      <c r="EM51" s="108"/>
+      <c r="EN51" s="108"/>
+      <c r="EO51" s="108"/>
+      <c r="EP51" s="109"/>
       <c r="EQ51" s="95"/>
       <c r="ER51" s="76"/>
       <c r="ES51" s="76"/>
@@ -10092,14 +10191,14 @@
       <c r="EF52" s="23"/>
       <c r="EG52" s="23"/>
       <c r="EH52" s="24"/>
-      <c r="EI52" s="27"/>
-      <c r="EJ52" s="23"/>
-      <c r="EK52" s="23"/>
-      <c r="EL52" s="23"/>
-      <c r="EM52" s="23"/>
-      <c r="EN52" s="23"/>
-      <c r="EO52" s="23"/>
-      <c r="EP52" s="24"/>
+      <c r="EI52" s="110"/>
+      <c r="EJ52" s="108"/>
+      <c r="EK52" s="108"/>
+      <c r="EL52" s="108"/>
+      <c r="EM52" s="108"/>
+      <c r="EN52" s="108"/>
+      <c r="EO52" s="108"/>
+      <c r="EP52" s="109"/>
       <c r="EQ52" s="95"/>
       <c r="ER52" s="76"/>
       <c r="ES52" s="76"/>
@@ -10118,8 +10217,8 @@
       <c r="FF52" s="94"/>
     </row>
     <row r="53" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A53" s="114"/>
-      <c r="B53" s="115"/>
+      <c r="A53" s="121"/>
+      <c r="B53" s="122"/>
       <c r="C53" s="8"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -10256,14 +10355,14 @@
       <c r="EF53" s="23"/>
       <c r="EG53" s="23"/>
       <c r="EH53" s="24"/>
-      <c r="EI53" s="27"/>
-      <c r="EJ53" s="23"/>
-      <c r="EK53" s="23"/>
-      <c r="EL53" s="23"/>
-      <c r="EM53" s="23"/>
-      <c r="EN53" s="23"/>
-      <c r="EO53" s="23"/>
-      <c r="EP53" s="24"/>
+      <c r="EI53" s="110"/>
+      <c r="EJ53" s="108"/>
+      <c r="EK53" s="108"/>
+      <c r="EL53" s="108"/>
+      <c r="EM53" s="108"/>
+      <c r="EN53" s="108"/>
+      <c r="EO53" s="108"/>
+      <c r="EP53" s="109"/>
       <c r="EQ53" s="95"/>
       <c r="ER53" s="76"/>
       <c r="ES53" s="76"/>
@@ -10282,8 +10381,8 @@
       <c r="FF53" s="94"/>
     </row>
     <row r="54" spans="1:163" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="116"/>
-      <c r="B54" s="117"/>
+      <c r="A54" s="123"/>
+      <c r="B54" s="124"/>
       <c r="C54" s="11"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -10420,14 +10519,14 @@
       <c r="EF54" s="19"/>
       <c r="EG54" s="19"/>
       <c r="EH54" s="20"/>
-      <c r="EI54" s="99"/>
-      <c r="EJ54" s="19"/>
-      <c r="EK54" s="19"/>
-      <c r="EL54" s="19"/>
-      <c r="EM54" s="19"/>
-      <c r="EN54" s="19"/>
-      <c r="EO54" s="19"/>
-      <c r="EP54" s="20"/>
+      <c r="EI54" s="111"/>
+      <c r="EJ54" s="112"/>
+      <c r="EK54" s="112"/>
+      <c r="EL54" s="112"/>
+      <c r="EM54" s="112"/>
+      <c r="EN54" s="112"/>
+      <c r="EO54" s="112"/>
+      <c r="EP54" s="113"/>
       <c r="EQ54" s="96"/>
       <c r="ER54" s="97"/>
       <c r="ES54" s="97"/>
@@ -10446,8 +10545,8 @@
       <c r="FF54" s="98"/>
     </row>
     <row r="55" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A55" s="118"/>
-      <c r="B55" s="118"/>
+      <c r="A55" s="125"/>
+      <c r="B55" s="125"/>
       <c r="C55" s="31"/>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
@@ -10611,8 +10710,8 @@
       <c r="FG55" s="100"/>
     </row>
     <row r="56" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A56" s="110"/>
-      <c r="B56" s="110"/>
+      <c r="A56" s="117"/>
+      <c r="B56" s="117"/>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
@@ -10776,8 +10875,8 @@
       <c r="FG56" s="100"/>
     </row>
     <row r="57" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A57" s="110"/>
-      <c r="B57" s="110"/>
+      <c r="A57" s="117"/>
+      <c r="B57" s="117"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
@@ -10941,8 +11040,8 @@
       <c r="FG57" s="100"/>
     </row>
     <row r="58" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A58" s="110"/>
-      <c r="B58" s="110"/>
+      <c r="A58" s="117"/>
+      <c r="B58" s="117"/>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
       <c r="E58" s="31"/>
@@ -11106,8 +11205,8 @@
       <c r="FG58" s="100"/>
     </row>
     <row r="59" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A59" s="110"/>
-      <c r="B59" s="110"/>
+      <c r="A59" s="117"/>
+      <c r="B59" s="117"/>
       <c r="C59" s="31"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
@@ -11271,8 +11370,8 @@
       <c r="FG59" s="100"/>
     </row>
     <row r="60" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A60" s="110"/>
-      <c r="B60" s="110"/>
+      <c r="A60" s="117"/>
+      <c r="B60" s="117"/>
       <c r="C60" s="31"/>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
@@ -11436,8 +11535,8 @@
       <c r="FG60" s="100"/>
     </row>
     <row r="61" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A61" s="110"/>
-      <c r="B61" s="110"/>
+      <c r="A61" s="117"/>
+      <c r="B61" s="117"/>
       <c r="C61" s="31"/>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
@@ -11601,8 +11700,8 @@
       <c r="FG61" s="100"/>
     </row>
     <row r="62" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A62" s="118"/>
-      <c r="B62" s="118"/>
+      <c r="A62" s="125"/>
+      <c r="B62" s="125"/>
       <c r="C62" s="31"/>
       <c r="D62" s="31"/>
       <c r="E62" s="31"/>
@@ -11766,8 +11865,8 @@
       <c r="FG62" s="100"/>
     </row>
     <row r="63" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A63" s="110"/>
-      <c r="B63" s="110"/>
+      <c r="A63" s="117"/>
+      <c r="B63" s="117"/>
       <c r="C63" s="31"/>
       <c r="D63" s="31"/>
       <c r="E63" s="31"/>
@@ -11931,8 +12030,8 @@
       <c r="FG63" s="100"/>
     </row>
     <row r="64" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A64" s="110"/>
-      <c r="B64" s="110"/>
+      <c r="A64" s="117"/>
+      <c r="B64" s="117"/>
       <c r="C64" s="31"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31"/>
@@ -12096,8 +12195,8 @@
       <c r="FG64" s="100"/>
     </row>
     <row r="65" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A65" s="110"/>
-      <c r="B65" s="110"/>
+      <c r="A65" s="117"/>
+      <c r="B65" s="117"/>
       <c r="C65" s="31"/>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
@@ -12261,8 +12360,8 @@
       <c r="FG65" s="100"/>
     </row>
     <row r="66" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A66" s="110"/>
-      <c r="B66" s="110"/>
+      <c r="A66" s="117"/>
+      <c r="B66" s="117"/>
       <c r="C66" s="31"/>
       <c r="D66" s="31"/>
       <c r="E66" s="31"/>
@@ -12426,8 +12525,8 @@
       <c r="FG66" s="100"/>
     </row>
     <row r="67" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A67" s="110"/>
-      <c r="B67" s="110"/>
+      <c r="A67" s="117"/>
+      <c r="B67" s="117"/>
       <c r="C67" s="31"/>
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
@@ -12591,8 +12690,8 @@
       <c r="FG67" s="100"/>
     </row>
     <row r="68" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A68" s="118"/>
-      <c r="B68" s="118"/>
+      <c r="A68" s="125"/>
+      <c r="B68" s="125"/>
       <c r="C68" s="31"/>
       <c r="D68" s="31"/>
       <c r="E68" s="31"/>
@@ -12756,8 +12855,8 @@
       <c r="FG68" s="100"/>
     </row>
     <row r="69" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A69" s="110"/>
-      <c r="B69" s="110"/>
+      <c r="A69" s="117"/>
+      <c r="B69" s="117"/>
       <c r="C69" s="31"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
@@ -12921,8 +13020,8 @@
       <c r="FG69" s="100"/>
     </row>
     <row r="70" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A70" s="110"/>
-      <c r="B70" s="110"/>
+      <c r="A70" s="117"/>
+      <c r="B70" s="117"/>
       <c r="C70" s="31"/>
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
@@ -13086,8 +13185,8 @@
       <c r="FG70" s="100"/>
     </row>
     <row r="71" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A71" s="110"/>
-      <c r="B71" s="110"/>
+      <c r="A71" s="117"/>
+      <c r="B71" s="117"/>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
@@ -13251,8 +13350,8 @@
       <c r="FG71" s="100"/>
     </row>
     <row r="72" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A72" s="110"/>
-      <c r="B72" s="110"/>
+      <c r="A72" s="117"/>
+      <c r="B72" s="117"/>
       <c r="C72" s="31"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
@@ -13416,8 +13515,8 @@
       <c r="FG72" s="100"/>
     </row>
     <row r="73" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A73" s="110"/>
-      <c r="B73" s="110"/>
+      <c r="A73" s="117"/>
+      <c r="B73" s="117"/>
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
@@ -13581,8 +13680,8 @@
       <c r="FG73" s="100"/>
     </row>
     <row r="74" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A74" s="110"/>
-      <c r="B74" s="110"/>
+      <c r="A74" s="117"/>
+      <c r="B74" s="117"/>
       <c r="C74" s="31"/>
       <c r="D74" s="31"/>
       <c r="E74" s="31"/>
@@ -13746,8 +13845,8 @@
       <c r="FG74" s="100"/>
     </row>
     <row r="75" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A75" s="118"/>
-      <c r="B75" s="118"/>
+      <c r="A75" s="125"/>
+      <c r="B75" s="125"/>
       <c r="C75" s="31"/>
       <c r="D75" s="31"/>
       <c r="E75" s="31"/>
@@ -13911,8 +14010,8 @@
       <c r="FG75" s="100"/>
     </row>
     <row r="76" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A76" s="110"/>
-      <c r="B76" s="110"/>
+      <c r="A76" s="117"/>
+      <c r="B76" s="117"/>
       <c r="C76" s="31"/>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
@@ -14076,8 +14175,8 @@
       <c r="FG76" s="100"/>
     </row>
     <row r="77" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A77" s="110"/>
-      <c r="B77" s="110"/>
+      <c r="A77" s="117"/>
+      <c r="B77" s="117"/>
       <c r="C77" s="31"/>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
@@ -14241,8 +14340,8 @@
       <c r="FG77" s="100"/>
     </row>
     <row r="78" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A78" s="110"/>
-      <c r="B78" s="110"/>
+      <c r="A78" s="117"/>
+      <c r="B78" s="117"/>
       <c r="C78" s="31"/>
       <c r="D78" s="31"/>
       <c r="E78" s="31"/>
@@ -14406,8 +14505,8 @@
       <c r="FG78" s="100"/>
     </row>
     <row r="79" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A79" s="110"/>
-      <c r="B79" s="110"/>
+      <c r="A79" s="117"/>
+      <c r="B79" s="117"/>
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
@@ -14571,8 +14670,8 @@
       <c r="FG79" s="100"/>
     </row>
     <row r="80" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A80" s="110"/>
-      <c r="B80" s="110"/>
+      <c r="A80" s="117"/>
+      <c r="B80" s="117"/>
       <c r="C80" s="31"/>
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
@@ -14736,8 +14835,8 @@
       <c r="FG80" s="100"/>
     </row>
     <row r="81" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A81" s="118"/>
-      <c r="B81" s="118"/>
+      <c r="A81" s="125"/>
+      <c r="B81" s="125"/>
       <c r="C81" s="31"/>
       <c r="D81" s="31"/>
       <c r="E81" s="31"/>
@@ -14901,8 +15000,8 @@
       <c r="FG81" s="100"/>
     </row>
     <row r="82" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A82" s="110"/>
-      <c r="B82" s="110"/>
+      <c r="A82" s="117"/>
+      <c r="B82" s="117"/>
       <c r="C82" s="31"/>
       <c r="D82" s="31"/>
       <c r="E82" s="31"/>
@@ -15066,8 +15165,8 @@
       <c r="FG82" s="100"/>
     </row>
     <row r="83" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A83" s="110"/>
-      <c r="B83" s="110"/>
+      <c r="A83" s="117"/>
+      <c r="B83" s="117"/>
       <c r="C83" s="31"/>
       <c r="D83" s="31"/>
       <c r="E83" s="31"/>
@@ -15231,8 +15330,8 @@
       <c r="FG83" s="100"/>
     </row>
     <row r="84" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A84" s="110"/>
-      <c r="B84" s="110"/>
+      <c r="A84" s="117"/>
+      <c r="B84" s="117"/>
       <c r="C84" s="31"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
@@ -15396,8 +15495,8 @@
       <c r="FG84" s="100"/>
     </row>
     <row r="85" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A85" s="110"/>
-      <c r="B85" s="110"/>
+      <c r="A85" s="117"/>
+      <c r="B85" s="117"/>
       <c r="C85" s="31"/>
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
@@ -15561,8 +15660,8 @@
       <c r="FG85" s="100"/>
     </row>
     <row r="86" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A86" s="110"/>
-      <c r="B86" s="110"/>
+      <c r="A86" s="117"/>
+      <c r="B86" s="117"/>
       <c r="C86" s="31"/>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
@@ -15726,8 +15825,8 @@
       <c r="FG86" s="100"/>
     </row>
     <row r="87" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A87" s="110"/>
-      <c r="B87" s="110"/>
+      <c r="A87" s="117"/>
+      <c r="B87" s="117"/>
       <c r="C87" s="31"/>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
@@ -15891,8 +15990,8 @@
       <c r="FG87" s="100"/>
     </row>
     <row r="88" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A88" s="110"/>
-      <c r="B88" s="110"/>
+      <c r="A88" s="117"/>
+      <c r="B88" s="117"/>
       <c r="C88" s="31"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
@@ -16056,8 +16155,8 @@
       <c r="FG88" s="100"/>
     </row>
     <row r="89" spans="1:163" x14ac:dyDescent="0.2">
-      <c r="A89" s="110"/>
-      <c r="B89" s="110"/>
+      <c r="A89" s="117"/>
+      <c r="B89" s="117"/>
       <c r="C89" s="31"/>
       <c r="D89" s="31"/>
       <c r="E89" s="31"/>

</xml_diff>